<commit_message>
functions + code cleanup
</commit_message>
<xml_diff>
--- a/pilot_project_distance_matrix.xlsx
+++ b/pilot_project_distance_matrix.xlsx
@@ -72,2173 +72,3277 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>896.5829791501653</v>
+        <v>738.0698469823274</v>
       </c>
       <c r="B1" t="n">
-        <v>895.8345204431964</v>
+        <v>774.296100927659</v>
       </c>
       <c r="C1" t="n">
-        <v>895.7646770333906</v>
+        <v>722.5153949281005</v>
       </c>
       <c r="D1" t="n">
-        <v>891.5574177227902</v>
+        <v>724.9867036523696</v>
       </c>
       <c r="E1" t="n">
-        <v>875.9818595770967</v>
+        <v>715.973750623445</v>
       </c>
       <c r="F1" t="n">
-        <v>847.4795279287611</v>
+        <v>709.080418826199</v>
       </c>
       <c r="G1" t="n">
-        <v>816.3882234867452</v>
+        <v>699.771205922132</v>
       </c>
       <c r="H1" t="n">
-        <v>786.2032350131968</v>
+        <v>1424.472650757128</v>
       </c>
       <c r="I1" t="n">
-        <v>718.0529448349589</v>
+        <v>1410.693716805984</v>
       </c>
       <c r="J1" t="n">
-        <v>644.8457757193253</v>
+        <v>1422.4231155811046</v>
       </c>
       <c r="K1" t="n">
-        <v>605.823833356971</v>
+        <v>1414.1790041439078</v>
       </c>
       <c r="L1" t="n">
-        <v>319.3567723492869</v>
+        <v>1432.3037198701743</v>
       </c>
       <c r="M1" t="n">
-        <v>389.5260975687312</v>
+        <v>746.9194259180172</v>
       </c>
       <c r="N1" t="n">
-        <v>424.66617242707304</v>
+        <v>708.7341060158003</v>
       </c>
       <c r="O1" t="n">
-        <v>424.5468935007972</v>
+        <v>733.1526789343056</v>
       </c>
       <c r="P1" t="n">
-        <v>583.8781784742998</v>
+        <v>703.7506524219849</v>
       </c>
       <c r="Q1" t="n">
-        <v>565.0798568233871</v>
+        <v>672.1067020306562</v>
       </c>
       <c r="R1" t="n">
-        <v>506.7034944714032</v>
+        <v>700.3044624217105</v>
       </c>
       <c r="S1" t="n">
-        <v>470.48984484624697</v>
+        <v>704.7848180918653</v>
       </c>
       <c r="T1" t="n">
-        <v>464.8512706074133</v>
+        <v>710.7989927530566</v>
       </c>
       <c r="U1" t="n">
-        <v>219.74940725122104</v>
+        <v>1258.8613127739825</v>
       </c>
       <c r="V1" t="n">
-        <v>235.4878660227978</v>
+        <v>1367.587589808462</v>
       </c>
       <c r="W1" t="n">
-        <v>239.14218192688475</v>
+        <v>1372.532439995936</v>
       </c>
       <c r="X1" t="n">
-        <v>226.9376984983128</v>
+        <v>1377.0056286768224</v>
       </c>
       <c r="Y1" t="n">
-        <v>228.39671461882673</v>
+        <v>1356.63052296297</v>
       </c>
       <c r="Z1" t="n">
-        <v>228.559624275484</v>
+        <v>901.7906217200954</v>
       </c>
       <c r="AA1" t="n">
-        <v>224.13680999437656</v>
+        <v>688.6779454796358</v>
       </c>
       <c r="AB1" t="n">
-        <v>220.9567115461861</v>
+        <v>683.3348417800765</v>
       </c>
       <c r="AC1" t="n">
-        <v>219.4539553113268</v>
+        <v>710.4095435424122</v>
       </c>
       <c r="AD1" t="n">
-        <v>213.05293479463595</v>
+        <v>688.2027177978662</v>
       </c>
       <c r="AE1" t="n">
-        <v>213.94914093227524</v>
+        <v>711.1818413025496</v>
       </c>
       <c r="AF1" t="n">
-        <v>218.77676034472</v>
+        <v>691.9714328116798</v>
       </c>
       <c r="AG1" t="n">
-        <v>228.21582877739237</v>
+        <v>689.518894053912</v>
       </c>
       <c r="AH1" t="n">
-        <v>236.94584425052687</v>
+        <v>840.9660636966337</v>
       </c>
       <c r="AI1" t="n">
-        <v>236.71813235667673</v>
+        <v>1389.0233623092934</v>
       </c>
       <c r="AJ1" t="n">
-        <v>279.91461807465976</v>
+        <v>1380.7679401420276</v>
       </c>
       <c r="AK1" t="n">
-        <v>296.21538049446644</v>
+        <v>1387.7195102323494</v>
       </c>
       <c r="AL1" t="n">
-        <v>297.3781090574743</v>
+        <v>1392.205125968645</v>
       </c>
       <c r="AM1" t="n">
-        <v>292.15881458826436</v>
+        <v>1324.2295579402353</v>
       </c>
       <c r="AN1" t="n">
-        <v>289.9319346764271</v>
+        <v>735.0620274966001</v>
       </c>
       <c r="AO1" t="n">
-        <v>245.96349861547225</v>
+        <v>714.9190393650861</v>
       </c>
       <c r="AP1" t="n">
-        <v>438.54712639607</v>
+        <v>731.2548636144616</v>
       </c>
       <c r="AQ1" t="n">
-        <v>482.75093853241725</v>
+        <v>702.5334670035868</v>
       </c>
       <c r="AR1" t="n">
-        <v>482.59381996833906</v>
+        <v>693.9560689966572</v>
       </c>
       <c r="AS1" t="n">
-        <v>483.52197516330585</v>
+        <v>718.3361057351226</v>
       </c>
       <c r="AT1" t="n">
-        <v>481.5667704563234</v>
+        <v>689.2599719435991</v>
       </c>
       <c r="AU1" t="n">
-        <v>287.81025195382625</v>
+        <v>714.5372785860982</v>
       </c>
       <c r="AV1" t="n">
-        <v>217.10159083353057</v>
+        <v>1458.7497883589729</v>
       </c>
       <c r="AW1" t="n">
-        <v>327.1011827095732</v>
+        <v>1450.849155584439</v>
       </c>
       <c r="AX1" t="n">
-        <v>345.03378036716236</v>
+        <v>1466.943432116595</v>
       </c>
       <c r="AY1" t="n">
-        <v>360.7084715306984</v>
+        <v>1467.9524064754717</v>
       </c>
       <c r="AZ1" t="n">
-        <v>374.5318550194773</v>
+        <v>1461.3893725805056</v>
       </c>
       <c r="BA1" t="n">
-        <v>372.91425828773197</v>
+        <v>691.589160185121</v>
       </c>
       <c r="BB1" t="n">
-        <v>305.9490547742824</v>
+        <v>689.9986576826082</v>
       </c>
       <c r="BC1" t="n">
-        <v>308.02281362939715</v>
+        <v>680.5445089267728</v>
       </c>
       <c r="BD1" t="n">
-        <v>304.5213845252625</v>
+        <v>689.9476109149767</v>
       </c>
       <c r="BE1" t="n">
-        <v>307.6542284051845</v>
+        <v>656.2679271075868</v>
       </c>
       <c r="BF1" t="n">
-        <v>318.1906290251718</v>
+        <v>696.7247594999236</v>
       </c>
       <c r="BG1" t="n">
-        <v>320.1037043162734</v>
+        <v>661.5010969184652</v>
       </c>
       <c r="BH1" t="n">
-        <v>586.1333913635675</v>
+        <v>669.2868997696363</v>
       </c>
       <c r="BI1" t="n">
-        <v>612.6888077602048</v>
+        <v>1034.4208943416347</v>
       </c>
       <c r="BJ1" t="n">
-        <v>613.4280925019062</v>
+        <v>1334.6362965351643</v>
       </c>
       <c r="BK1" t="n">
-        <v>609.174661974907</v>
+        <v>1335.1570009795337</v>
       </c>
       <c r="BL1" t="n">
-        <v>617.1161546434994</v>
+        <v>1331.5625401695945</v>
       </c>
       <c r="BM1" t="n">
-        <v>427.98049010740453</v>
+        <v>1328.5608144892296</v>
       </c>
       <c r="BN1" t="n">
-        <v>458.43885193529337</v>
+        <v>1097.0973410101146</v>
       </c>
       <c r="BO1" t="n">
-        <v>487.83297149026</v>
+        <v>690.1642593547524</v>
       </c>
       <c r="BP1" t="n">
-        <v>547.1071979798069</v>
+        <v>703.7855913578258</v>
       </c>
       <c r="BQ1" t="n">
-        <v>1036.0596201122294</v>
+        <v>699.5960960139583</v>
       </c>
       <c r="BR1" t="n">
-        <v>1136.311289020631</v>
+        <v>703.5901244883238</v>
       </c>
       <c r="BS1" t="n">
-        <v>779.9617936140439</v>
+        <v>705.4697773934284</v>
       </c>
       <c r="BT1" t="n">
-        <v>689.151341147388</v>
+        <v>704.3623999761958</v>
       </c>
       <c r="BU1" t="n">
-        <v>757.4102394785345</v>
+        <v>681.5186632749457</v>
       </c>
       <c r="BV1" t="n">
-        <v>812.9700605042823</v>
+        <v>979.6082477226212</v>
       </c>
       <c r="BW1" t="n">
-        <v>879.9812897520496</v>
+        <v>1358.6544915947077</v>
       </c>
       <c r="BX1" t="n">
-        <v>959.2860039609069</v>
+        <v>1363.8905958029252</v>
       </c>
       <c r="BY1" t="n">
-        <v>983.3767056825693</v>
+        <v>1385.9503534582016</v>
       </c>
       <c r="BZ1" t="n">
-        <v>908.9833055911522</v>
+        <v>1365.4301780276107</v>
       </c>
       <c r="CA1" t="n">
-        <v>820.4818043070068</v>
+        <v>1204.5950074700486</v>
       </c>
       <c r="CB1" t="n">
-        <v>697.5162543521584</v>
+        <v>718.3578559455366</v>
       </c>
       <c r="CC1" t="n">
-        <v>493.9787064538949</v>
+        <v>709.9588981504584</v>
       </c>
       <c r="CD1" t="n">
-        <v>250.01256908041583</v>
+        <v>728.541060631691</v>
       </c>
       <c r="CE1" t="n">
-        <v>223.843132674099</v>
+        <v>726.6804936864913</v>
       </c>
       <c r="CF1" t="n">
-        <v>219.60336380685322</v>
+        <v>712.921931309983</v>
       </c>
       <c r="CG1" t="n">
-        <v>242.60125814181856</v>
+        <v>696.4673101134013</v>
       </c>
       <c r="CH1" t="n">
-        <v>240.40464342854762</v>
+        <v>682.5963656385103</v>
       </c>
       <c r="CI1" t="n">
-        <v>229.63679252772639</v>
+        <v>673.0342548417717</v>
       </c>
       <c r="CJ1" t="n">
-        <v>222.97296487713746</v>
+        <v>1463.9187834140248</v>
       </c>
       <c r="CK1" t="n">
-        <v>218.9239838413232</v>
+        <v>1455.4401352170075</v>
       </c>
       <c r="CL1" t="n">
-        <v>190.4124185135845</v>
+        <v>1502.8341886469782</v>
       </c>
       <c r="CM1" t="n">
-        <v>203.75201833310723</v>
+        <v>1519.409196724342</v>
       </c>
       <c r="CN1" t="n">
-        <v>228.59312890980203</v>
+        <v>1526.6387877022814</v>
       </c>
       <c r="CO1" t="n">
-        <v>1224.3782230051636</v>
+        <v>844.7022417453782</v>
       </c>
       <c r="CP1" t="n">
-        <v>346.0833729306782</v>
+        <v>831.6352994813828</v>
       </c>
       <c r="CQ1" t="n">
-        <v>218.6604599176191</v>
+        <v>793.2095652042868</v>
       </c>
       <c r="CR1" t="n">
-        <v>233.88358406393888</v>
+        <v>718.0217667972436</v>
       </c>
       <c r="CS1" t="n">
-        <v>232.8615270583432</v>
+        <v>719.3581892439946</v>
       </c>
       <c r="CT1" t="n">
-        <v>222.45601562794624</v>
+        <v>730.1764543438992</v>
       </c>
       <c r="CU1" t="n">
-        <v>219.5858759058966</v>
+        <v>720.4599578765818</v>
       </c>
       <c r="CV1" t="n">
-        <v>222.64640492864527</v>
+        <v>717.573078407951</v>
       </c>
       <c r="CW1" t="n">
-        <v>210.7374847160358</v>
+        <v>1435.3566408941326</v>
       </c>
       <c r="CX1" t="n">
-        <v>219.9012630085152</v>
+        <v>1436.7524186187175</v>
       </c>
       <c r="CY1" t="n">
-        <v>212.4054645687997</v>
+        <v>1445.1685289357602</v>
       </c>
       <c r="CZ1" t="n">
-        <v>211.7361867410593</v>
+        <v>1446.8934039829012</v>
       </c>
       <c r="DA1" t="n">
-        <v>212.66276928401257</v>
+        <v>1430.337928072848</v>
       </c>
       <c r="DB1" t="n">
-        <v>739.7621854762303</v>
+        <v>746.261528896076</v>
       </c>
       <c r="DC1" t="n">
-        <v>1112.4060802892268</v>
+        <v>702.8546082934944</v>
       </c>
       <c r="DD1" t="n">
-        <v>1113.7068292743495</v>
+        <v>689.0622335604321</v>
       </c>
       <c r="DE1" t="n">
-        <v>854.9973476593667</v>
+        <v>728.6430503396026</v>
       </c>
       <c r="DF1" t="n">
-        <v>193.20337301073795</v>
+        <v>702.8550718996722</v>
       </c>
       <c r="DG1" t="n">
-        <v>189.61877324169734</v>
+        <v>719.8550635996473</v>
       </c>
       <c r="DH1" t="n">
-        <v>188.6576327695245</v>
+        <v>692.0262210291496</v>
       </c>
       <c r="DI1" t="n">
-        <v>396.33866310750795</v>
+        <v>676.833759282607</v>
       </c>
       <c r="DJ1" t="n">
-        <v>498.4351166127244</v>
+        <v>808.9152987917729</v>
       </c>
       <c r="DK1" t="n">
-        <v>501.8659922593213</v>
+        <v>1436.0910494548182</v>
       </c>
       <c r="DL1" t="n">
-        <v>502.9759416094227</v>
+        <v>1428.5677055388935</v>
       </c>
       <c r="DM1" t="n">
-        <v>504.2215174306809</v>
+        <v>1443.5882900848712</v>
       </c>
       <c r="DN1" t="n">
-        <v>359.11024755462347</v>
+        <v>1437.9048556846872</v>
       </c>
       <c r="DO1" t="n">
-        <v>207.95282818646268</v>
+        <v>1381.7109881754811</v>
       </c>
       <c r="DP1" t="n">
-        <v>210.88863827835263</v>
+        <v>739.3345206929748</v>
       </c>
       <c r="DQ1" t="n">
-        <v>212.6836683656646</v>
+        <v>736.2992115338433</v>
       </c>
       <c r="DR1" t="n">
-        <v>216.07437131106147</v>
+        <v>737.7655851925756</v>
       </c>
       <c r="DS1" t="n">
-        <v>215.02529310771718</v>
+        <v>735.353840288401</v>
       </c>
       <c r="DT1" t="n">
-        <v>219.04114203563552</v>
+        <v>720.792294392171</v>
       </c>
       <c r="DU1" t="n">
-        <v>216.81527036091154</v>
+        <v>721.5038507397</v>
       </c>
       <c r="DV1" t="n">
-        <v>214.45474246425425</v>
+        <v>683.6032418979645</v>
       </c>
       <c r="DW1" t="n">
-        <v>242.1838539994434</v>
+        <v>698.7981603870711</v>
       </c>
       <c r="DX1" t="n">
-        <v>239.34410096712415</v>
+        <v>1413.5734706597398</v>
       </c>
       <c r="DY1" t="n">
-        <v>227.00755173183026</v>
+        <v>1417.5308741380227</v>
       </c>
       <c r="DZ1" t="n">
-        <v>227.8652929959532</v>
+        <v>1435.6473333809902</v>
       </c>
       <c r="EA1" t="n">
-        <v>225.43695648900405</v>
+        <v>1436.204070784635</v>
       </c>
       <c r="EB1" t="n">
-        <v>196.1744990455769</v>
+        <v>1439.8112085465975</v>
       </c>
       <c r="EC1" t="n">
-        <v>207.2133419181</v>
+        <v>723.2787355314654</v>
       </c>
       <c r="ED1" t="n">
-        <v>240.83233332682875</v>
+        <v>709.5566243430981</v>
       </c>
       <c r="EE1" t="n">
-        <v>249.907058344143</v>
+        <v>694.3486585362816</v>
       </c>
       <c r="EF1" t="n">
-        <v>294.2503376124656</v>
+        <v>693.4951846036946</v>
       </c>
       <c r="EG1" t="n">
-        <v>366.0625675624167</v>
+        <v>665.1267792534454</v>
       </c>
       <c r="EH1" t="n">
-        <v>427.9485980120899</v>
+        <v>701.7729844871168</v>
       </c>
       <c r="EI1" t="n">
-        <v>511.90259224905446</v>
+        <v>677.2615906557721</v>
       </c>
       <c r="EJ1" t="n">
-        <v>774.9064886580206</v>
+        <v>689.8441773572362</v>
       </c>
       <c r="EK1" t="n">
-        <v>937.2645425567698</v>
+        <v>1319.0645909443472</v>
       </c>
       <c r="EL1" t="n">
-        <v>938.328072160928</v>
+        <v>1476.5232104678141</v>
       </c>
       <c r="EM1" t="n">
-        <v>937.5541808865838</v>
+        <v>1484.7151541430508</v>
       </c>
       <c r="EN1" t="n">
-        <v>913.5627064327732</v>
+        <v>1470.6097686646156</v>
       </c>
       <c r="EO1" t="n">
-        <v>727.7377486129745</v>
+        <v>1466.0499723995213</v>
       </c>
       <c r="EP1" t="n">
-        <v>478.2315362498464</v>
+        <v>983.9481903430324</v>
       </c>
       <c r="EQ1" t="n">
-        <v>423.50333955287283</v>
+        <v>700.0256339654646</v>
       </c>
       <c r="ER1" t="n">
-        <v>356.1491673065587</v>
+        <v>693.9407981810502</v>
       </c>
       <c r="ES1" t="n">
-        <v>275.0246985936032</v>
+        <v>697.3507081198516</v>
       </c>
       <c r="ET1" t="n">
-        <v>189.38532674751494</v>
+        <v>702.7542228555369</v>
       </c>
       <c r="EU1" t="n">
-        <v>183.94081613565723</v>
+        <v>702.7578650559711</v>
       </c>
       <c r="EV1" t="n">
-        <v>189.63485637073285</v>
+        <v>710.4626789503112</v>
       </c>
       <c r="EW1" t="n">
-        <v>189.1307254507615</v>
+        <v>686.8644133349094</v>
       </c>
       <c r="EX1" t="n">
-        <v>193.33144286571962</v>
+        <v>1047.0328474873452</v>
       </c>
       <c r="EY1" t="n">
-        <v>196.86177525642415</v>
+        <v>1487.6763567011399</v>
       </c>
       <c r="EZ1" t="n">
-        <v>199.33031322780627</v>
+        <v>1495.3900983758635</v>
       </c>
       <c r="FA1" t="n">
-        <v>404.95117243492365</v>
+        <v>1510.807141292777</v>
       </c>
       <c r="FB1" t="n">
-        <v>849.0451351634157</v>
+        <v>1497.6836398560092</v>
       </c>
       <c r="FC1" t="n">
-        <v>859.46022241277</v>
+        <v>1302.295061835231</v>
       </c>
       <c r="FD1" t="n">
-        <v>789.0750365642643</v>
+        <v>703.1887968337062</v>
       </c>
       <c r="FE1" t="n">
-        <v>279.6420722476182</v>
+        <v>681.4856049325551</v>
       </c>
       <c r="FF1" t="n">
-        <v>283.8800002572317</v>
+        <v>694.1489167603362</v>
       </c>
       <c r="FG1" t="n">
-        <v>296.08456848813745</v>
+        <v>693.1023252113166</v>
       </c>
       <c r="FH1" t="n">
-        <v>475.25111777580526</v>
+        <v>681.9106676118834</v>
       </c>
       <c r="FI1" t="n">
-        <v>617.2166182585195</v>
+        <v>701.1358128639757</v>
       </c>
       <c r="FJ1" t="n">
-        <v>613.813945703612</v>
+        <v>697.2876513871709</v>
       </c>
       <c r="FK1" t="n">
-        <v>615.3213913980409</v>
+        <v>713.4999038355719</v>
       </c>
       <c r="FL1" t="n">
-        <v>606.3652757459125</v>
+        <v>1485.9878372522871</v>
       </c>
       <c r="FM1" t="n">
-        <v>469.1623046459288</v>
+        <v>1471.396078190548</v>
       </c>
       <c r="FN1" t="n">
-        <v>256.5049314482066</v>
+        <v>1489.6600191100845</v>
       </c>
       <c r="FO1" t="n">
-        <v>251.19717734137748</v>
+        <v>1478.2944959980155</v>
       </c>
       <c r="FP1" t="n">
-        <v>248.01753060332538</v>
+        <v>1470.9721331593576</v>
       </c>
       <c r="FQ1" t="n">
-        <v>247.0390683590352</v>
+        <v>726.0160963562865</v>
       </c>
       <c r="FR1" t="n">
-        <v>252.5881515921634</v>
+        <v>715.5004357394243</v>
       </c>
       <c r="FS1" t="n">
-        <v>300.389833937576</v>
+        <v>709.5641405188885</v>
       </c>
       <c r="FT1" t="n">
-        <v>347.50175345446775</v>
+        <v>684.5098476076237</v>
       </c>
       <c r="FU1" t="n">
-        <v>389.0990334934641</v>
+        <v>691.9004467867802</v>
       </c>
       <c r="FV1" t="n">
-        <v>429.54529955086167</v>
+        <v>703.7586786389362</v>
       </c>
       <c r="FW1" t="n">
-        <v>472.0396604009163</v>
+        <v>696.3561043370202</v>
       </c>
       <c r="FX1" t="n">
-        <v>499.3038110841901</v>
+        <v>690.4568022812507</v>
       </c>
       <c r="FY1" t="n">
-        <v>524.078552278394</v>
+        <v>1288.7989801420417</v>
       </c>
       <c r="FZ1" t="n">
-        <v>546.4746350428499</v>
+        <v>1484.5466966804659</v>
       </c>
       <c r="GA1" t="n">
-        <v>566.5623655172112</v>
+        <v>1487.5825981383055</v>
       </c>
       <c r="GB1" t="n">
-        <v>574.4997412949655</v>
+        <v>1496.9926831901932</v>
       </c>
       <c r="GC1" t="n">
-        <v>532.395400848656</v>
+        <v>1479.253420471265</v>
       </c>
       <c r="GD1" t="n">
-        <v>476.04955725612206</v>
+        <v>1037.4523235258262</v>
       </c>
       <c r="GE1" t="n">
-        <v>409.1301619299384</v>
+        <v>675.0882143774512</v>
       </c>
       <c r="GF1" t="n">
-        <v>327.5394770729246</v>
+        <v>667.6208343073445</v>
       </c>
       <c r="GG1" t="n">
-        <v>229.0717115087378</v>
+        <v>696.7706292893533</v>
       </c>
       <c r="GH1" t="n">
-        <v>210.68601587346765</v>
+        <v>686.9525691754442</v>
       </c>
       <c r="GI1" t="n">
-        <v>199.5216784943415</v>
+        <v>689.3611643264567</v>
       </c>
       <c r="GJ1" t="n">
-        <v>757.8168504003777</v>
+        <v>682.4015157005311</v>
       </c>
       <c r="GK1" t="n">
-        <v>902.9840769384662</v>
+        <v>686.717564115721</v>
       </c>
       <c r="GL1" t="n">
-        <v>566.8068903514834</v>
+        <v>1405.3484229069154</v>
       </c>
       <c r="GM1" t="n">
-        <v>484.3941344668979</v>
+        <v>1719.581733253174</v>
       </c>
       <c r="GN1" t="n">
-        <v>386.7596560994392</v>
+        <v>1707.650517965686</v>
       </c>
       <c r="GO1" t="n">
-        <v>382.8820944531399</v>
+        <v>1718.570690214593</v>
       </c>
       <c r="GP1" t="n">
-        <v>617.0413991737645</v>
+        <v>1715.4611483369363</v>
       </c>
       <c r="GQ1" t="n">
-        <v>1073.982811134534</v>
+        <v>1210.283908953217</v>
       </c>
       <c r="GR1" t="n">
-        <v>1077.571968333834</v>
+        <v>705.246253275848</v>
       </c>
       <c r="GS1" t="n">
-        <v>1083.7964296947443</v>
+        <v>688.5482229988097</v>
       </c>
       <c r="GT1" t="n">
-        <v>1082.587045322895</v>
+        <v>694.6488183135198</v>
       </c>
       <c r="GU1" t="n">
-        <v>406.4226449185819</v>
+        <v>660.2624211206022</v>
       </c>
       <c r="GV1" t="n">
-        <v>399.71159180180734</v>
+        <v>648.5561493498692</v>
       </c>
       <c r="GW1" t="n">
-        <v>378.24040420133446</v>
+        <v>675.709290261492</v>
       </c>
       <c r="GX1" t="n">
-        <v>486.14320903543853</v>
+        <v>665.3764577016253</v>
       </c>
       <c r="GY1" t="n">
-        <v>575.6939907670078</v>
+        <v>688.8768033994996</v>
       </c>
       <c r="GZ1" t="n">
-        <v>576.7571154093966</v>
+        <v>1561.2148020514633</v>
       </c>
       <c r="HA1" t="n">
-        <v>601.0862686854532</v>
+        <v>1561.922016005951</v>
       </c>
       <c r="HB1" t="n">
-        <v>645.3995769150654</v>
+        <v>1573.1142171144982</v>
       </c>
       <c r="HC1" t="n">
-        <v>626.2698312806751</v>
+        <v>1574.4738466256886</v>
       </c>
       <c r="HD1" t="n">
-        <v>611.7248269862044</v>
+        <v>1569.93641333684</v>
       </c>
       <c r="HE1" t="n">
-        <v>342.8865202211445</v>
+        <v>711.4798155877431</v>
       </c>
       <c r="HF1" t="n">
-        <v>221.5325341223644</v>
+        <v>692.4956495151323</v>
       </c>
       <c r="HG1" t="n">
-        <v>256.71776225291205</v>
+        <v>695.074704710945</v>
       </c>
       <c r="HH1" t="n">
-        <v>260.8901610310541</v>
+        <v>719.4743275524852</v>
       </c>
       <c r="HI1" t="n">
-        <v>304.88549385997277</v>
+        <v>671.3024182795975</v>
       </c>
       <c r="HJ1" t="n">
-        <v>315.2369102666362</v>
+        <v>708.1256860194392</v>
       </c>
       <c r="HK1" t="n">
-        <v>320.4368966793848</v>
+        <v>668.2698374545</v>
       </c>
       <c r="HL1" t="n">
-        <v>290.0799261175512</v>
+        <v>657.1999320756265</v>
       </c>
       <c r="HM1" t="n">
-        <v>286.8065907909886</v>
+        <v>1558.1666249196576</v>
       </c>
       <c r="HN1" t="n">
-        <v>241.03032308901956</v>
+        <v>1564.3127188457468</v>
       </c>
       <c r="HO1" t="n">
-        <v>227.27009369156215</v>
+        <v>1564.6267928644695</v>
       </c>
       <c r="HP1" t="n">
-        <v>240.0284210833971</v>
+        <v>1566.903753027553</v>
       </c>
       <c r="HQ1" t="n">
-        <v>252.72014173202643</v>
+        <v>1572.363691225616</v>
       </c>
       <c r="HR1" t="n">
-        <v>275.9090515976501</v>
+        <v>728.0639797455196</v>
       </c>
       <c r="HS1" t="n">
-        <v>297.3616438202459</v>
+        <v>716.4409419583435</v>
       </c>
       <c r="HT1" t="n">
-        <v>313.0606833754543</v>
+        <v>710.2256383793232</v>
       </c>
       <c r="HU1" t="n">
-        <v>561.178981264928</v>
+        <v>719.5930080200443</v>
       </c>
       <c r="HV1" t="n">
-        <v>607.8707684562206</v>
+        <v>701.2042933964952</v>
       </c>
       <c r="HW1" t="n">
-        <v>617.6615213537133</v>
+        <v>690.0953520346734</v>
       </c>
       <c r="HX1" t="n">
-        <v>619.4010635330999</v>
+        <v>719.2206744696323</v>
       </c>
       <c r="HY1" t="n">
-        <v>619.7145617837684</v>
+        <v>668.6664403612582</v>
       </c>
       <c r="HZ1" t="n">
-        <v>408.64615533758166</v>
+        <v>1043.3381981967543</v>
       </c>
       <c r="IA1" t="n">
-        <v>344.7446081727237</v>
+        <v>1396.3738869348085</v>
       </c>
       <c r="IB1" t="n">
-        <v>336.1648270153439</v>
+        <v>1394.6104121519486</v>
       </c>
       <c r="IC1" t="n">
-        <v>331.6238367018683</v>
+        <v>1399.535010522767</v>
       </c>
       <c r="ID1" t="n">
-        <v>335.74003403227516</v>
+        <v>1397.8723560370074</v>
       </c>
       <c r="IE1" t="n">
-        <v>346.5679762373294</v>
+        <v>1178.24843942213</v>
       </c>
       <c r="IF1" t="n">
-        <v>336.1170839208349</v>
+        <v>684.0188789771827</v>
       </c>
       <c r="IG1" t="n">
-        <v>324.24228052865357</v>
+        <v>694.2154834929195</v>
       </c>
       <c r="IH1" t="n">
-        <v>323.7094748648498</v>
+        <v>718.8485637424861</v>
       </c>
       <c r="II1" t="n">
-        <v>311.97603340227136</v>
+        <v>720.2326598808689</v>
       </c>
       <c r="IJ1" t="n">
-        <v>292.6739126366129</v>
+        <v>702.285402430685</v>
       </c>
       <c r="IK1" t="n">
-        <v>290.6680953991602</v>
+        <v>755.8809157441419</v>
       </c>
       <c r="IL1" t="n">
-        <v>287.13949033734644</v>
+        <v>753.476268201067</v>
       </c>
       <c r="IM1" t="n">
-        <v>297.36537648571533</v>
+        <v>762.3769080887325</v>
       </c>
       <c r="IN1" t="n">
-        <v>306.1650443019389</v>
+        <v>1415.1621504407535</v>
       </c>
       <c r="IO1" t="n">
-        <v>309.2560873694995</v>
+        <v>1395.1556911025737</v>
       </c>
       <c r="IP1" t="n">
-        <v>328.85044934061295</v>
+        <v>1397.6485316408896</v>
       </c>
       <c r="IQ1" t="n">
-        <v>629.3628348741868</v>
+        <v>1387.17342100442</v>
       </c>
       <c r="IR1" t="n">
-        <v>713.2482432382305</v>
+        <v>1379.569216705271</v>
       </c>
       <c r="IS1" t="n">
-        <v>715.0667427058231</v>
+        <v>740.5875909490916</v>
       </c>
       <c r="IT1" t="n">
-        <v>714.6634273806068</v>
+        <v>751.2301619475551</v>
       </c>
       <c r="IU1" t="n">
-        <v>783.2350014825876</v>
+        <v>758.6617384557177</v>
       </c>
       <c r="IV1" t="n">
-        <v>874.9599989566732</v>
+        <v>723.2511344725347</v>
       </c>
       <c r="IW1" t="n">
-        <v>734.0226929351932</v>
+        <v>726.7253492929724</v>
       </c>
       <c r="IX1" t="n">
-        <v>317.97792975769426</v>
+        <v>747.159244597854</v>
       </c>
       <c r="IY1" t="n">
-        <v>322.74897181257376</v>
+        <v>730.2276656375482</v>
       </c>
       <c r="IZ1" t="n">
-        <v>322.10572698932856</v>
+        <v>682.5001036020557</v>
       </c>
       <c r="JA1" t="n">
-        <v>313.7711675022543</v>
+        <v>1568.7397406840948</v>
       </c>
       <c r="JB1" t="n">
-        <v>323.10041054281226</v>
+        <v>1577.2957696758551</v>
       </c>
       <c r="JC1" t="n">
-        <v>318.9000563980281</v>
+        <v>1570.840546049898</v>
       </c>
       <c r="JD1" t="n">
-        <v>318.9477249120046</v>
+        <v>1583.6795805280876</v>
       </c>
       <c r="JE1" t="n">
-        <v>321.7557702790605</v>
+        <v>1572.7411471344474</v>
       </c>
       <c r="JF1" t="n">
-        <v>320.1262001252424</v>
+        <v>751.2619154866229</v>
       </c>
       <c r="JG1" t="n">
-        <v>312.8065452757439</v>
+        <v>680.0278779505064</v>
       </c>
       <c r="JH1" t="n">
-        <v>319.47963360562505</v>
+        <v>694.8623118863632</v>
       </c>
       <c r="JI1" t="n">
-        <v>356.1018061123068</v>
+        <v>730.6386224048947</v>
       </c>
       <c r="JJ1" t="n">
-        <v>357.3241954963653</v>
+        <v>748.3662248183688</v>
       </c>
       <c r="JK1" t="n">
-        <v>356.771100331183</v>
+        <v>775.1957004535057</v>
       </c>
       <c r="JL1" t="n">
-        <v>355.892923421666</v>
+        <v>763.4018436696309</v>
       </c>
       <c r="JM1" t="n">
-        <v>347.55708972479385</v>
+        <v>751.6590779194048</v>
       </c>
       <c r="JN1" t="n">
-        <v>294.3324769143156</v>
+        <v>760.1824609931494</v>
       </c>
       <c r="JO1" t="n">
-        <v>281.04451697400106</v>
+        <v>740.727958412356</v>
       </c>
       <c r="JP1" t="n">
-        <v>264.8949185869945</v>
+        <v>670.6922419727853</v>
       </c>
       <c r="JQ1" t="n">
-        <v>250.60634032327053</v>
+        <v>713.9340121012342</v>
       </c>
       <c r="JR1" t="n">
-        <v>242.68801536810025</v>
+        <v>1609.1104003484013</v>
       </c>
       <c r="JS1" t="n">
-        <v>253.9677881056673</v>
+        <v>1587.4712728726522</v>
       </c>
       <c r="JT1" t="n">
-        <v>304.2315486307818</v>
+        <v>1606.4372445148263</v>
       </c>
       <c r="JU1" t="n">
-        <v>738.458816055964</v>
+        <v>1598.7829130203556</v>
       </c>
       <c r="JV1" t="n">
-        <v>750.9513522087966</v>
+        <v>1620.468932717505</v>
       </c>
       <c r="JW1" t="n">
-        <v>756.5798076255836</v>
+        <v>697.2801586505939</v>
       </c>
       <c r="JX1" t="n">
-        <v>749.6782923091748</v>
+        <v>739.8457986064564</v>
       </c>
       <c r="JY1" t="n">
-        <v>351.1370954512271</v>
+        <v>755.0642709034787</v>
       </c>
       <c r="JZ1" t="n">
-        <v>359.831430175538</v>
+        <v>753.4824375640471</v>
       </c>
       <c r="KA1" t="n">
-        <v>362.96610961821864</v>
+        <v>715.440168867972</v>
       </c>
       <c r="KB1" t="n">
-        <v>358.9585189240509</v>
+        <v>702.0096058760209</v>
       </c>
       <c r="KC1" t="n">
-        <v>351.6627326088666</v>
+        <v>689.8831022776255</v>
       </c>
       <c r="KD1" t="n">
-        <v>365.28951521554166</v>
+        <v>697.8182498618687</v>
       </c>
       <c r="KE1" t="n">
-        <v>374.0443125736964</v>
+        <v>1375.1556372330674</v>
       </c>
       <c r="KF1" t="n">
-        <v>379.41361694108934</v>
+        <v>1423.867411371463</v>
       </c>
       <c r="KG1" t="n">
-        <v>392.35030681743933</v>
+        <v>1427.0438900085614</v>
       </c>
       <c r="KH1" t="n">
-        <v>381.1370297660789</v>
+        <v>1420.5981951030724</v>
       </c>
       <c r="KI1" t="n">
-        <v>360.79031092906587</v>
+        <v>1422.21937851352</v>
       </c>
       <c r="KJ1" t="n">
-        <v>343.3476010614043</v>
+        <v>795.8095930395266</v>
       </c>
       <c r="KK1" t="n">
-        <v>340.6884410750465</v>
+        <v>671.5002697803443</v>
       </c>
       <c r="KL1" t="n">
-        <v>332.44615166619707</v>
+        <v>716.9142815628953</v>
       </c>
       <c r="KM1" t="n">
-        <v>333.41533466496804</v>
+        <v>685.4086900845348</v>
       </c>
       <c r="KN1" t="n">
-        <v>336.8894894892713</v>
+        <v>682.4203273942178</v>
       </c>
       <c r="KO1" t="n">
-        <v>639.1083549765389</v>
+        <v>1277.7780554421495</v>
       </c>
       <c r="KP1" t="n">
-        <v>683.4197933058023</v>
+        <v>1477.2103769407015</v>
       </c>
       <c r="KQ1" t="n">
-        <v>677.6397252852249</v>
+        <v>1481.940292723305</v>
       </c>
       <c r="KR1" t="n">
-        <v>677.7695192413956</v>
+        <v>1478.2750153859538</v>
       </c>
       <c r="KS1" t="n">
-        <v>858.5654515696712</v>
+        <v>1474.251268909898</v>
       </c>
       <c r="KT1" t="n">
-        <v>333.09040560806943</v>
+        <v>1036.8994990202823</v>
       </c>
       <c r="KU1" t="n">
-        <v>468.22688970682196</v>
+        <v>703.4284015257667</v>
       </c>
       <c r="KV1" t="n">
-        <v>521.5141043603111</v>
+        <v>664.414217948174</v>
       </c>
       <c r="KW1" t="n">
-        <v>526.3552892365748</v>
+        <v>714.5419369669362</v>
       </c>
       <c r="KX1" t="n">
-        <v>528.8350264982834</v>
+        <v>691.8855810233358</v>
       </c>
       <c r="KY1" t="n">
-        <v>530.6675378573049</v>
+        <v>688.6374151118839</v>
       </c>
       <c r="KZ1" t="n">
-        <v>398.1269229787669</v>
+        <v>714.128208452744</v>
       </c>
       <c r="LA1" t="n">
-        <v>318.8416206008457</v>
+        <v>701.6199855090807</v>
       </c>
       <c r="LB1" t="n">
-        <v>354.47888589986866</v>
+        <v>725.4359693227946</v>
       </c>
       <c r="LC1" t="n">
-        <v>356.07616641497424</v>
+        <v>1436.8560862168463</v>
       </c>
       <c r="LD1" t="n">
-        <v>353.22015366154415</v>
+        <v>1441.9211316805563</v>
       </c>
       <c r="LE1" t="n">
-        <v>350.31279016033454</v>
+        <v>1461.135897178493</v>
       </c>
       <c r="LF1" t="n">
-        <v>352.6593963634287</v>
+        <v>1457.5674312753797</v>
       </c>
       <c r="LG1" t="n">
-        <v>351.5963591595647</v>
+        <v>1445.8990549226974</v>
       </c>
       <c r="LH1" t="n">
-        <v>489.7801816430287</v>
+        <v>714.0848052626587</v>
       </c>
       <c r="LI1" t="n">
-        <v>588.3208045521316</v>
+        <v>699.4858154975419</v>
       </c>
       <c r="LJ1" t="n">
-        <v>661.3504749172661</v>
+        <v>688.918094022126</v>
       </c>
       <c r="LK1" t="n">
-        <v>726.7001706941096</v>
+        <v>698.0218553695534</v>
       </c>
       <c r="LL1" t="n">
-        <v>746.7159699287267</v>
+        <v>664.1065326754483</v>
       </c>
       <c r="LM1" t="n">
-        <v>705.2412914497323</v>
+        <v>701.8216666137184</v>
       </c>
       <c r="LN1" t="n">
-        <v>681.9919596075033</v>
+        <v>693.2780341705479</v>
       </c>
       <c r="LO1" t="n">
-        <v>666.7700367682534</v>
+        <v>697.5952323449601</v>
       </c>
       <c r="LP1" t="n">
-        <v>641.7102449718143</v>
+        <v>1440.0597935555836</v>
       </c>
       <c r="LQ1" t="n">
-        <v>697.7701183676813</v>
+        <v>1429.7952911990142</v>
       </c>
       <c r="LR1" t="n">
-        <v>638.8815421869318</v>
+        <v>1433.9990364407706</v>
       </c>
       <c r="LS1" t="n">
-        <v>580.939267645644</v>
+        <v>1412.1382360919729</v>
       </c>
       <c r="LT1" t="n">
-        <v>511.953689982917</v>
+        <v>1413.7620843032666</v>
       </c>
       <c r="LU1" t="n">
-        <v>466.2429347308473</v>
+        <v>696.2439382005261</v>
       </c>
       <c r="LV1" t="n">
-        <v>435.41720162388384</v>
+        <v>697.1376768289008</v>
       </c>
       <c r="LW1" t="n">
-        <v>390.00873103818867</v>
+        <v>707.0794873982061</v>
       </c>
       <c r="LX1" t="n">
-        <v>392.60462100264374</v>
+        <v>708.8143616628356</v>
       </c>
       <c r="LY1" t="n">
-        <v>429.1046515563109</v>
+        <v>707.8362240702949</v>
       </c>
       <c r="LZ1" t="n">
-        <v>465.1304994482733</v>
+        <v>709.0774037219508</v>
       </c>
       <c r="MA1" t="n">
-        <v>489.41076129726656</v>
+        <v>708.0750218112898</v>
       </c>
       <c r="MB1" t="n">
-        <v>510.6127252993297</v>
+        <v>678.129510784372</v>
       </c>
       <c r="MC1" t="n">
-        <v>553.6514248055354</v>
+        <v>1365.9852261205474</v>
       </c>
       <c r="MD1" t="n">
-        <v>564.9271680211993</v>
+        <v>1394.9935996343675</v>
       </c>
       <c r="ME1" t="n">
-        <v>575.0460801029411</v>
+        <v>1392.2095808425129</v>
       </c>
       <c r="MF1" t="n">
-        <v>624.1620516480904</v>
+        <v>1405.5792260201426</v>
       </c>
       <c r="MG1" t="n">
-        <v>978.4918178870533</v>
+        <v>1391.589644874208</v>
       </c>
       <c r="MH1" t="n">
-        <v>817.1202061566776</v>
+        <v>788.2793436270772</v>
       </c>
       <c r="MI1" t="n">
-        <v>813.0317490400681</v>
+        <v>680.4802208160484</v>
       </c>
       <c r="MJ1" t="n">
-        <v>814.6884612215686</v>
+        <v>681.5759532517981</v>
       </c>
       <c r="MK1" t="n">
-        <v>644.384750402722</v>
+        <v>714.9531171362167</v>
       </c>
       <c r="ML1" t="n">
-        <v>361.5043369952535</v>
+        <v>714.363233619265</v>
       </c>
       <c r="MM1" t="n">
-        <v>341.21552275546077</v>
+        <v>699.0904671375977</v>
       </c>
       <c r="MN1" t="n">
-        <v>342.76151505937315</v>
+        <v>708.9814831062133</v>
       </c>
       <c r="MO1" t="n">
-        <v>306.1851672121539</v>
+        <v>694.861176143546</v>
       </c>
       <c r="MP1" t="n">
-        <v>286.63644820494335</v>
+        <v>1471.793606708395</v>
       </c>
       <c r="MQ1" t="n">
-        <v>276.01995396827044</v>
+        <v>1911.3376802138996</v>
       </c>
       <c r="MR1" t="n">
-        <v>281.0026329395093</v>
+        <v>1909.8935235618476</v>
       </c>
       <c r="MS1" t="n">
-        <v>312.4058515699519</v>
+        <v>1914.985295019979</v>
       </c>
       <c r="MT1" t="n">
-        <v>310.3071601830117</v>
+        <v>1913.2886976955083</v>
       </c>
       <c r="MU1" t="n">
-        <v>309.7355022897563</v>
+        <v>1410.6920105762665</v>
       </c>
       <c r="MV1" t="n">
-        <v>303.08640528546874</v>
+        <v>745.4781283262331</v>
       </c>
       <c r="MW1" t="n">
-        <v>301.8770114876554</v>
+        <v>707.7555661179833</v>
       </c>
       <c r="MX1" t="n">
-        <v>260.4605662121972</v>
+        <v>766.8432488577712</v>
       </c>
       <c r="MY1" t="n">
-        <v>267.75015148334</v>
+        <v>729.9494476901028</v>
       </c>
       <c r="MZ1" t="n">
-        <v>287.32840531179573</v>
+        <v>755.7559493832532</v>
       </c>
       <c r="NA1" t="n">
-        <v>299.2263788121426</v>
+        <v>797.580693954633</v>
       </c>
       <c r="NB1" t="n">
-        <v>319.42683332642923</v>
+        <v>800.182582874438</v>
       </c>
       <c r="NC1" t="n">
-        <v>335.94000739855636</v>
+        <v>777.9234544870175</v>
       </c>
       <c r="ND1" t="n">
-        <v>348.6344331278348</v>
+        <v>1635.6630564738086</v>
       </c>
       <c r="NE1" t="n">
-        <v>343.7285486062493</v>
+        <v>1615.6200933415423</v>
       </c>
       <c r="NF1" t="n">
-        <v>347.8468026509811</v>
+        <v>1609.5062271314257</v>
       </c>
       <c r="NG1" t="n">
-        <v>352.68437265854783</v>
+        <v>1606.2062532529155</v>
       </c>
       <c r="NH1" t="n">
-        <v>843.2321648682017</v>
+        <v>1587.4061127676803</v>
       </c>
       <c r="NI1" t="n">
-        <v>832.4128403044502</v>
+        <v>711.5444904590363</v>
       </c>
       <c r="NJ1" t="n">
-        <v>327.8388280029113</v>
+        <v>671.1386094019741</v>
       </c>
       <c r="NK1" t="n">
-        <v>260.7262726740538</v>
+        <v>691.0238979445456</v>
       </c>
       <c r="NL1" t="n">
-        <v>266.96628699357484</v>
+        <v>709.4396040679688</v>
       </c>
       <c r="NM1" t="n">
-        <v>263.01874472848755</v>
+        <v>689.495221142083</v>
       </c>
       <c r="NN1" t="n">
-        <v>278.9876899994312</v>
+        <v>704.8059383016099</v>
       </c>
       <c r="NO1" t="n">
-        <v>283.83387851048695</v>
+        <v>694.4138214972953</v>
       </c>
       <c r="NP1" t="n">
-        <v>297.81147980884685</v>
+        <v>666.6817786495064</v>
       </c>
       <c r="NQ1" t="n">
-        <v>294.03784731314187</v>
+        <v>1659.285182593096</v>
       </c>
       <c r="NR1" t="n">
-        <v>300.74031945616986</v>
+        <v>1710.7782717742346</v>
       </c>
       <c r="NS1" t="n">
-        <v>290.8218807150103</v>
+        <v>1710.760789115855</v>
       </c>
       <c r="NT1" t="n">
-        <v>290.73102605581624</v>
+        <v>1709.9737735339452</v>
       </c>
       <c r="NU1" t="n">
-        <v>286.6047727502049</v>
+        <v>1705.2558930830178</v>
       </c>
       <c r="NV1" t="n">
-        <v>285.3122233294207</v>
+        <v>807.7855285662699</v>
       </c>
       <c r="NW1" t="n">
-        <v>280.1380064875631</v>
+        <v>697.2473533188388</v>
       </c>
       <c r="NX1" t="n">
-        <v>278.26222951975444</v>
+        <v>665.3715597995246</v>
       </c>
       <c r="NY1" t="n">
-        <v>376.6867272778778</v>
+        <v>714.1702716682418</v>
       </c>
       <c r="NZ1" t="n">
-        <v>538.6008381397128</v>
+        <v>684.6443188224282</v>
       </c>
       <c r="OA1" t="n">
-        <v>538.4602129041313</v>
+        <v>683.6648840818316</v>
       </c>
       <c r="OB1" t="n">
-        <v>538.9188935002144</v>
+        <v>719.0071873804943</v>
       </c>
       <c r="OC1" t="n">
-        <v>620.5881694995558</v>
+        <v>693.9850187616295</v>
       </c>
       <c r="OD1" t="n">
-        <v>828.5205396960233</v>
+        <v>783.6528271307257</v>
       </c>
       <c r="OE1" t="n">
-        <v>732.5626317634163</v>
+        <v>1549.4701572264705</v>
       </c>
       <c r="OF1" t="n">
-        <v>746.9415757718841</v>
+        <v>1551.5956964844254</v>
       </c>
       <c r="OG1" t="n">
-        <v>747.5934454391715</v>
+        <v>1560.0406094257653</v>
       </c>
       <c r="OH1" t="n">
-        <v>675.2845472030839</v>
+        <v>1559.791847565605</v>
       </c>
       <c r="OI1" t="n">
-        <v>299.82952241707426</v>
+        <v>1519.6482440192003</v>
       </c>
       <c r="OJ1" t="n">
-        <v>300.47426973516133</v>
+        <v>704.9780249162383</v>
       </c>
       <c r="OK1" t="n">
-        <v>258.9775267991151</v>
+        <v>690.9308046044641</v>
       </c>
       <c r="OL1" t="n">
-        <v>244.8975873026405</v>
+        <v>687.5978044160081</v>
       </c>
       <c r="OM1" t="n">
-        <v>249.01813227761272</v>
+        <v>696.2152324499061</v>
       </c>
       <c r="ON1" t="n">
-        <v>229.1895783948324</v>
+        <v>696.9746092211274</v>
       </c>
       <c r="OO1" t="n">
-        <v>217.9088463886393</v>
+        <v>712.6115761838461</v>
       </c>
       <c r="OP1" t="n">
-        <v>219.13825579898463</v>
+        <v>709.9622516370423</v>
       </c>
       <c r="OQ1" t="n">
-        <v>331.6935354118507</v>
+        <v>748.1203847133157</v>
       </c>
       <c r="OR1" t="n">
-        <v>503.349839209073</v>
+        <v>1780.0134545253425</v>
       </c>
       <c r="OS1" t="n">
-        <v>633.2211870245709</v>
+        <v>1759.1846751803287</v>
       </c>
       <c r="OT1" t="n">
-        <v>752.5267283975267</v>
+        <v>1776.9036550929854</v>
       </c>
       <c r="OU1" t="n">
-        <v>874.2172866215395</v>
+        <v>1760.906770784535</v>
       </c>
       <c r="OV1" t="n">
-        <v>927.5417851826077</v>
+        <v>1750.0356217497363</v>
       </c>
       <c r="OW1" t="n">
-        <v>933.354341175936</v>
+        <v>739.6095936957851</v>
       </c>
       <c r="OX1" t="n">
-        <v>946.3888173940496</v>
+        <v>739.788181612343</v>
       </c>
       <c r="OY1" t="n">
-        <v>944.4346819009266</v>
+        <v>719.5682246414225</v>
       </c>
       <c r="OZ1" t="n">
-        <v>931.7639489068151</v>
+        <v>723.4657384031497</v>
       </c>
       <c r="PA1" t="n">
-        <v>933.4162775608098</v>
+        <v>696.6299300402013</v>
       </c>
       <c r="PB1" t="n">
-        <v>934.2655674565882</v>
+        <v>680.7632538056998</v>
       </c>
       <c r="PC1" t="n">
-        <v>925.5832386795199</v>
+        <v>690.0248272182579</v>
       </c>
       <c r="PD1" t="n">
-        <v>923.8457123292825</v>
+        <v>662.806730982631</v>
       </c>
       <c r="PE1" t="n">
-        <v>895.273746615351</v>
+        <v>705.693244349017</v>
       </c>
       <c r="PF1" t="n">
-        <v>1021.1713305601273</v>
+        <v>691.2651395509095</v>
       </c>
       <c r="PG1" t="n">
-        <v>1221.2362780398153</v>
+        <v>709.6039063971559</v>
       </c>
       <c r="PH1" t="n">
-        <v>891.5775781842391</v>
+        <v>855.4148960567235</v>
       </c>
       <c r="PI1" t="n">
-        <v>444.3592817550555</v>
+        <v>1602.616435134409</v>
       </c>
       <c r="PJ1" t="n">
-        <v>399.4675845274948</v>
+        <v>1609.4659156031576</v>
       </c>
       <c r="PK1" t="n">
-        <v>344.3672286324649</v>
+        <v>1595.5617559884681</v>
       </c>
       <c r="PL1" t="n">
-        <v>279.57201987517135</v>
+        <v>1589.6945803763253</v>
       </c>
       <c r="PM1" t="n">
-        <v>223.8415755616427</v>
+        <v>1539.815679339221</v>
       </c>
       <c r="PN1" t="n">
-        <v>210.6069895847519</v>
+        <v>716.82921776307</v>
       </c>
       <c r="PO1" t="n">
-        <v>217.79046624638153</v>
+        <v>699.0121431001166</v>
       </c>
       <c r="PP1" t="n">
-        <v>218.7714560488422</v>
+        <v>732.431026797302</v>
       </c>
       <c r="PQ1" t="n">
-        <v>247.6282316896136</v>
+        <v>732.947293560849</v>
       </c>
       <c r="PR1" t="n">
-        <v>245.4918450186594</v>
+        <v>737.7752304000761</v>
       </c>
       <c r="PS1" t="n">
-        <v>235.3847262366286</v>
+        <v>741.6309096054865</v>
       </c>
       <c r="PT1" t="n">
-        <v>236.0706836643245</v>
+        <v>730.0410451626216</v>
       </c>
       <c r="PU1" t="n">
-        <v>245.92210485296516</v>
+        <v>745.7620645094272</v>
       </c>
       <c r="PV1" t="n">
-        <v>219.6523275598904</v>
+        <v>712.2014688310354</v>
       </c>
       <c r="PW1" t="n">
-        <v>263.02311726702254</v>
+        <v>696.9632664040062</v>
       </c>
       <c r="PX1" t="n">
-        <v>399.85390630279363</v>
+        <v>735.0914619360758</v>
       </c>
       <c r="PY1" t="n">
-        <v>332.016153094003</v>
+        <v>1480.412460187502</v>
       </c>
       <c r="PZ1" t="n">
-        <v>438.6321988409143</v>
+        <v>1667.2192282719875</v>
       </c>
       <c r="QA1" t="n">
-        <v>521.123752285496</v>
+        <v>1658.3837401911208</v>
       </c>
       <c r="QB1" t="n">
-        <v>593.904389943282</v>
+        <v>1664.7382359297774</v>
       </c>
       <c r="QC1" t="n">
-        <v>656.5262800102594</v>
+        <v>1680.524888551495</v>
       </c>
       <c r="QD1" t="n">
-        <v>677.1851897674484</v>
+        <v>1066.9367478272143</v>
       </c>
       <c r="QE1" t="n">
-        <v>679.3391354164905</v>
+        <v>746.2388521204634</v>
       </c>
       <c r="QF1" t="n">
-        <v>680.5642092615425</v>
+        <v>754.7816597113466</v>
       </c>
       <c r="QG1" t="n">
-        <v>681.1104540919141</v>
+        <v>738.2503463042082</v>
       </c>
       <c r="QH1" t="n">
-        <v>682.0822999838815</v>
+        <v>722.5800112283177</v>
       </c>
       <c r="QI1" t="n">
-        <v>679.6460553063536</v>
+        <v>715.9725529944436</v>
       </c>
       <c r="QJ1" t="n">
-        <v>679.0241002214813</v>
+        <v>685.4810684291995</v>
       </c>
       <c r="QK1" t="n">
-        <v>679.9335048409099</v>
+        <v>723.4837420811059</v>
       </c>
       <c r="QL1" t="n">
-        <v>682.2569116910398</v>
+        <v>695.6967170560683</v>
       </c>
       <c r="QM1" t="n">
-        <v>689.3584754379096</v>
+        <v>703.9360415100864</v>
       </c>
       <c r="QN1" t="n">
-        <v>691.6546268712901</v>
+        <v>745.5247538498534</v>
       </c>
       <c r="QO1" t="n">
-        <v>724.907127963715</v>
+        <v>726.639035451657</v>
       </c>
       <c r="QP1" t="n">
-        <v>745.6784706004325</v>
+        <v>1922.168339082832</v>
       </c>
       <c r="QQ1" t="n">
-        <v>744.0872971108315</v>
+        <v>1913.6450812062042</v>
       </c>
       <c r="QR1" t="n">
-        <v>746.3404029047402</v>
+        <v>1905.9679481734418</v>
       </c>
       <c r="QS1" t="n">
-        <v>690.6196906937892</v>
+        <v>1908.7396826225677</v>
       </c>
       <c r="QT1" t="n">
-        <v>586.4710704801087</v>
+        <v>1909.442470981238</v>
       </c>
       <c r="QU1" t="n">
-        <v>549.5623253357895</v>
+        <v>686.9090801256535</v>
       </c>
       <c r="QV1" t="n">
-        <v>547.5020147961073</v>
+        <v>710.6291399538549</v>
       </c>
       <c r="QW1" t="n">
-        <v>607.7914248285729</v>
+        <v>698.1534417760512</v>
       </c>
       <c r="QX1" t="n">
-        <v>619.5710143488702</v>
+        <v>733.7486420386937</v>
       </c>
       <c r="QY1" t="n">
-        <v>624.3842453206922</v>
+        <v>737.0574301876472</v>
       </c>
       <c r="QZ1" t="n">
-        <v>624.3717947560156</v>
+        <v>716.208894528022</v>
       </c>
       <c r="RA1" t="n">
-        <v>627.7816305913001</v>
+        <v>734.7087715218792</v>
       </c>
       <c r="RB1" t="n">
-        <v>653.2062934007146</v>
+        <v>724.0692821977163</v>
       </c>
       <c r="RC1" t="n">
-        <v>657.5247318098536</v>
+        <v>1755.1159289220107</v>
       </c>
       <c r="RD1" t="n">
-        <v>661.2766790438709</v>
+        <v>1946.1646194431423</v>
       </c>
       <c r="RE1" t="n">
-        <v>661.8460266429902</v>
+        <v>1936.5548496343442</v>
       </c>
       <c r="RF1" t="n">
-        <v>668.5696948277231</v>
+        <v>1940.2481145815493</v>
       </c>
       <c r="RG1" t="n">
-        <v>645.2022679588479</v>
+        <v>1930.4172492546138</v>
       </c>
       <c r="RH1" t="n">
-        <v>642.4465360179643</v>
+        <v>1059.0909419469883</v>
       </c>
       <c r="RI1" t="n">
-        <v>648.061235470453</v>
+        <v>697.461778968335</v>
       </c>
       <c r="RJ1" t="n">
-        <v>661.4555786182382</v>
+        <v>694.9578316347371</v>
       </c>
       <c r="RK1" t="n">
-        <v>678.035998910472</v>
+        <v>695.8912234680503</v>
       </c>
       <c r="RL1" t="n">
-        <v>1081.659455103302</v>
+        <v>704.354026679666</v>
       </c>
       <c r="RM1" t="n">
-        <v>1111.7545904936958</v>
+        <v>696.962513497438</v>
       </c>
       <c r="RN1" t="n">
-        <v>1075.9040515437898</v>
+        <v>696.3231383177557</v>
       </c>
       <c r="RO1" t="n">
-        <v>423.91303330037414</v>
+        <v>710.9209729149159</v>
       </c>
       <c r="RP1" t="n">
-        <v>211.10172318955077</v>
+        <v>897.422012541323</v>
       </c>
       <c r="RQ1" t="n">
-        <v>205.87372701611645</v>
+        <v>1914.0554881146477</v>
       </c>
       <c r="RR1" t="n">
-        <v>219.44712320946857</v>
+        <v>1904.2697713522439</v>
       </c>
       <c r="RS1" t="n">
-        <v>215.32237671765665</v>
+        <v>1906.0948592121733</v>
       </c>
       <c r="RT1" t="n">
-        <v>209.19810618267203</v>
+        <v>1918.7314436679314</v>
       </c>
       <c r="RU1" t="n">
-        <v>211.41056866504945</v>
+        <v>1817.8949969716166</v>
       </c>
       <c r="RV1" t="n">
-        <v>214.62361417886106</v>
+        <v>719.4743109908466</v>
       </c>
       <c r="RW1" t="n">
-        <v>199.4885640527202</v>
+        <v>699.7792725425959</v>
       </c>
       <c r="RX1" t="n">
-        <v>197.54797318787612</v>
+        <v>695.228556761916</v>
       </c>
       <c r="RY1" t="n">
-        <v>215.6390478192345</v>
+        <v>704.1285238041409</v>
       </c>
       <c r="RZ1" t="n">
-        <v>214.51729993972918</v>
+        <v>704.3210146600723</v>
       </c>
       <c r="SA1" t="n">
-        <v>215.97039151094998</v>
+        <v>692.5079675298645</v>
       </c>
       <c r="SB1" t="n">
-        <v>217.1397203235122</v>
+        <v>710.9479406878097</v>
       </c>
       <c r="SC1" t="n">
-        <v>221.91617994697026</v>
+        <v>699.5315324098682</v>
       </c>
       <c r="SD1" t="n">
-        <v>213.1534614180839</v>
+        <v>1803.8596475050686</v>
       </c>
       <c r="SE1" t="n">
-        <v>219.32458510888097</v>
+        <v>1803.0652282334831</v>
       </c>
       <c r="SF1" t="n">
-        <v>225.88397992856753</v>
+        <v>1787.1885245307085</v>
       </c>
       <c r="SG1" t="n">
-        <v>228.68939488236296</v>
+        <v>1799.903653607394</v>
       </c>
       <c r="SH1" t="n">
-        <v>232.78654715800718</v>
+        <v>1785.9870586415136</v>
       </c>
       <c r="SI1" t="n">
-        <v>230.94009520889068</v>
+        <v>671.9380973216323</v>
       </c>
       <c r="SJ1" t="n">
-        <v>232.3556463389759</v>
+        <v>708.7412009038371</v>
       </c>
       <c r="SK1" t="n">
-        <v>249.2617254942917</v>
+        <v>712.5413253075774</v>
       </c>
       <c r="SL1" t="n">
-        <v>410.4188290822819</v>
+        <v>911.266005285176</v>
       </c>
       <c r="SM1" t="n">
-        <v>453.9279084931638</v>
+        <v>1306.6301206768808</v>
       </c>
       <c r="SN1" t="n">
-        <v>761.6041424259918</v>
+        <v>1296.7367783247607</v>
       </c>
       <c r="SO1" t="n">
-        <v>761.3844262838186</v>
+        <v>1315.4621580679009</v>
       </c>
       <c r="SP1" t="n">
-        <v>694.0962748627967</v>
+        <v>1309.2220397066585</v>
       </c>
       <c r="SQ1" t="n">
-        <v>670.9118759413211</v>
+        <v>1653.4713008811286</v>
       </c>
       <c r="SR1" t="n">
-        <v>295.4177711738056</v>
+        <v>1708.4449372477497</v>
       </c>
       <c r="SS1" t="n">
-        <v>299.2984508922297</v>
+        <v>1701.004679948295</v>
       </c>
       <c r="ST1" t="n">
-        <v>301.2969931134155</v>
+        <v>1700.5442817800747</v>
       </c>
       <c r="SU1" t="n">
-        <v>303.3620686998495</v>
+        <v>1711.6433117905149</v>
       </c>
       <c r="SV1" t="n">
-        <v>304.47593649007666</v>
+        <v>1231.8140743932418</v>
       </c>
       <c r="SW1" t="n">
-        <v>301.79898331551453</v>
+        <v>711.5561392852209</v>
       </c>
       <c r="SX1" t="n">
-        <v>301.62955497203774</v>
+        <v>692.0889737626234</v>
       </c>
       <c r="SY1" t="n">
-        <v>311.1695308874004</v>
+        <v>689.3929827940719</v>
       </c>
       <c r="SZ1" t="n">
-        <v>307.2735497116669</v>
+        <v>713.9679661427709</v>
       </c>
       <c r="TA1" t="n">
-        <v>298.0028772517701</v>
+        <v>709.6418721091275</v>
       </c>
       <c r="TB1" t="n">
-        <v>293.7790233725144</v>
+        <v>736.2121576042813</v>
       </c>
       <c r="TC1" t="n">
-        <v>326.548664371837</v>
+        <v>720.4662547480964</v>
       </c>
       <c r="TD1" t="n">
-        <v>411.0535847876682</v>
+        <v>780.9982466439963</v>
       </c>
       <c r="TE1" t="n">
-        <v>406.07965791324995</v>
+        <v>1775.9751497102661</v>
       </c>
       <c r="TF1" t="n">
-        <v>418.4540702429507</v>
+        <v>1775.7131374991882</v>
       </c>
       <c r="TG1" t="n">
-        <v>440.6347079297691</v>
+        <v>1760.448717389657</v>
       </c>
       <c r="TH1" t="n">
-        <v>528.9678914669875</v>
+        <v>1766.5153641152206</v>
       </c>
       <c r="TI1" t="n">
-        <v>459.80798782358903</v>
+        <v>1730.1360558643314</v>
       </c>
       <c r="TJ1" t="n">
-        <v>462.53467715955253</v>
+        <v>695.9478498771459</v>
       </c>
       <c r="TK1" t="n">
-        <v>518.4092180314312</v>
+        <v>694.3475998376591</v>
       </c>
       <c r="TL1" t="n">
-        <v>541.8196466643377</v>
+        <v>655.7782811438124</v>
       </c>
       <c r="TM1" t="n">
-        <v>436.8202592791726</v>
+        <v>706.3944079698917</v>
       </c>
       <c r="TN1" t="n">
-        <v>435.0133459054948</v>
+        <v>693.9443076651922</v>
       </c>
       <c r="TO1" t="n">
-        <v>433.6306148644323</v>
+        <v>670.3143509493716</v>
       </c>
       <c r="TP1" t="n">
-        <v>345.9508392485141</v>
+        <v>712.8394603799268</v>
       </c>
       <c r="TQ1" t="n">
-        <v>272.32464719009124</v>
+        <v>718.1411346724675</v>
       </c>
       <c r="TR1" t="n">
-        <v>267.999963452422</v>
+        <v>1724.8023457839354</v>
       </c>
       <c r="TS1" t="n">
-        <v>276.60232259358344</v>
+        <v>1714.7638190490961</v>
       </c>
       <c r="TT1" t="n">
-        <v>278.7792317920209</v>
+        <v>1719.8511848726696</v>
       </c>
       <c r="TU1" t="n">
-        <v>287.90863637641377</v>
+        <v>1729.437798541629</v>
       </c>
       <c r="TV1" t="n">
-        <v>289.90487741418815</v>
+        <v>1727.0085547424933</v>
       </c>
       <c r="TW1" t="n">
-        <v>289.2061721495463</v>
+        <v>705.4660394058941</v>
       </c>
       <c r="TX1" t="n">
-        <v>285.1054398068487</v>
+        <v>712.3424694625131</v>
       </c>
       <c r="TY1" t="n">
-        <v>279.00637726960804</v>
+        <v>693.7010076577895</v>
       </c>
       <c r="TZ1" t="n">
-        <v>273.78547304676346</v>
+        <v>684.0217767368086</v>
       </c>
       <c r="UA1" t="n">
-        <v>273.24296444114583</v>
+        <v>697.7304021300754</v>
       </c>
       <c r="UB1" t="n">
-        <v>271.60596060816744</v>
+        <v>658.9502748645298</v>
       </c>
       <c r="UC1" t="n">
-        <v>263.169764237535</v>
+        <v>699.8643367529262</v>
       </c>
       <c r="UD1" t="n">
-        <v>264.9230892248045</v>
+        <v>652.036834808131</v>
       </c>
       <c r="UE1" t="n">
-        <v>261.31054914366484</v>
+        <v>1661.6266838592412</v>
       </c>
       <c r="UF1" t="n">
-        <v>255.26631832964185</v>
+        <v>1804.1838947722565</v>
       </c>
       <c r="UG1" t="n">
-        <v>248.94708797186127</v>
+        <v>1801.01402083405</v>
       </c>
       <c r="UH1" t="n">
-        <v>287.3702337169662</v>
+        <v>1807.3461115778337</v>
       </c>
       <c r="UI1" t="n">
-        <v>288.1654469377614</v>
+        <v>1807.2333441624928</v>
       </c>
       <c r="UJ1" t="n">
-        <v>282.3103087461221</v>
+        <v>974.8986057577864</v>
       </c>
       <c r="UK1" t="n">
-        <v>272.2489093714237</v>
+        <v>724.2188104840828</v>
       </c>
       <c r="UL1" t="n">
-        <v>268.1525825342103</v>
+        <v>718.0100588286025</v>
       </c>
       <c r="UM1" t="n">
-        <v>230.40237170284252</v>
+        <v>715.4404981249232</v>
       </c>
       <c r="UN1" t="n">
-        <v>261.138344380251</v>
+        <v>717.3331901034317</v>
       </c>
       <c r="UO1" t="n">
-        <v>470.2064771685081</v>
+        <v>708.2730472590675</v>
       </c>
       <c r="UP1" t="n">
-        <v>503.98407436691764</v>
+        <v>707.7460777521509</v>
       </c>
       <c r="UQ1" t="n">
-        <v>503.558302297747</v>
+        <v>719.8956685763328</v>
       </c>
       <c r="UR1" t="n">
-        <v>504.6210975141837</v>
+        <v>932.323617727282</v>
       </c>
       <c r="US1" t="n">
-        <v>483.15544182359145</v>
+        <v>1960.7427024057358</v>
       </c>
       <c r="UT1" t="n">
-        <v>289.77638117733335</v>
+        <v>1945.6586831473874</v>
       </c>
       <c r="UU1" t="n">
-        <v>224.17607507789978</v>
+        <v>1943.5083465153991</v>
       </c>
       <c r="UV1" t="n">
-        <v>231.45453785519888</v>
+        <v>1954.2813265343432</v>
       </c>
       <c r="UW1" t="n">
-        <v>225.65927337044903</v>
+        <v>1843.3468500435029</v>
       </c>
       <c r="UX1" t="n">
-        <v>223.84063943525018</v>
+        <v>719.799928941804</v>
       </c>
       <c r="UY1" t="n">
-        <v>207.86454866163658</v>
+        <v>701.3639945337696</v>
       </c>
       <c r="UZ1" t="n">
-        <v>213.48069395121175</v>
+        <v>712.9810194095386</v>
       </c>
       <c r="VA1" t="n">
-        <v>206.80707039712033</v>
+        <v>738.0419688521238</v>
       </c>
       <c r="VB1" t="n">
-        <v>194.62726669616424</v>
+        <v>726.6516954902728</v>
       </c>
       <c r="VC1" t="n">
-        <v>196.88676821370308</v>
+        <v>692.6483528008386</v>
       </c>
       <c r="VD1" t="n">
-        <v>197.65413942980305</v>
+        <v>715.9187024262795</v>
       </c>
       <c r="VE1" t="n">
-        <v>210.27817259782438</v>
+        <v>683.2958677829031</v>
       </c>
       <c r="VF1" t="n">
-        <v>207.18053892166506</v>
+        <v>672.1813288127946</v>
       </c>
       <c r="VG1" t="n">
-        <v>284.5873668058591</v>
+        <v>689.6462522820384</v>
       </c>
       <c r="VH1" t="n">
-        <v>446.78427752734416</v>
+        <v>662.6093089255124</v>
       </c>
       <c r="VI1" t="n">
-        <v>539.7181694201157</v>
+        <v>1144.3365146208275</v>
       </c>
       <c r="VJ1" t="n">
-        <v>562.2155525909004</v>
+        <v>1388.8498654295609</v>
       </c>
       <c r="VK1" t="n">
-        <v>576.7348149717867</v>
+        <v>1406.8963068333262</v>
       </c>
       <c r="VL1" t="n">
-        <v>546.5228813159831</v>
+        <v>1421.283587066</v>
       </c>
       <c r="VM1" t="n">
-        <v>482.49947267300195</v>
+        <v>1436.7596064937925</v>
       </c>
       <c r="VN1" t="n">
-        <v>809.436418211436</v>
+        <v>1119.6715551521422</v>
       </c>
       <c r="VO1" t="n">
-        <v>829.9888114668497</v>
+        <v>769.7496575650367</v>
       </c>
       <c r="VP1" t="n">
-        <v>792.2362809218218</v>
+        <v>745.0396534921224</v>
       </c>
       <c r="VQ1" t="n">
-        <v>338.16835535781524</v>
+        <v>748.7448911612673</v>
       </c>
       <c r="VR1" t="n">
-        <v>197.97504221482083</v>
+        <v>706.8811755637606</v>
       </c>
       <c r="VS1" t="n">
-        <v>201.46869391802142</v>
+        <v>694.4241625545873</v>
       </c>
       <c r="VT1" t="n">
-        <v>199.3179061534715</v>
+        <v>687.5786511369516</v>
       </c>
       <c r="VU1" t="n">
-        <v>202.31248113555495</v>
+        <v>652.0254679447197</v>
       </c>
       <c r="VV1" t="n">
-        <v>210.62928777759586</v>
+        <v>998.4359629783078</v>
       </c>
       <c r="VW1" t="n">
-        <v>232.71438408460511</v>
+        <v>1723.4946300238723</v>
       </c>
       <c r="VX1" t="n">
-        <v>234.08910255435688</v>
+        <v>1702.5206400575441</v>
       </c>
       <c r="VY1" t="n">
-        <v>236.782401630068</v>
+        <v>1724.9720111003285</v>
       </c>
       <c r="VZ1" t="n">
-        <v>235.72653306561767</v>
+        <v>1713.7505254443581</v>
       </c>
       <c r="WA1" t="n">
-        <v>235.73295495889633</v>
+        <v>1547.5528018918174</v>
       </c>
       <c r="WB1" t="n">
-        <v>222.6118779033744</v>
+        <v>702.9751153952957</v>
       </c>
       <c r="WC1" t="n">
-        <v>331.78212125504405</v>
+        <v>703.5677881199945</v>
       </c>
       <c r="WD1" t="n">
-        <v>431.9177871748234</v>
+        <v>1086.831930150994</v>
       </c>
       <c r="WE1" t="n">
-        <v>494.4574738153754</v>
+        <v>1092.714809306723</v>
       </c>
       <c r="WF1" t="n">
-        <v>551.2679497951582</v>
+        <v>1082.365588734753</v>
       </c>
       <c r="WG1" t="n">
-        <v>602.7576265333435</v>
+        <v>1087.5084154402196</v>
       </c>
       <c r="WH1" t="n">
-        <v>607.4473570720503</v>
+        <v>1082.3269192205416</v>
       </c>
       <c r="WI1" t="n">
-        <v>612.3010358942004</v>
+        <v>1809.077882412487</v>
       </c>
       <c r="WJ1" t="n">
-        <v>625.635406839759</v>
+        <v>2319.528470689443</v>
       </c>
       <c r="WK1" t="n">
-        <v>627.9587711849786</v>
+        <v>2324.301610025738</v>
       </c>
       <c r="WL1" t="n">
-        <v>630.163898675058</v>
+        <v>2333.5232911922885</v>
       </c>
       <c r="WM1" t="n">
-        <v>624.0124057141719</v>
+        <v>2343.4433485376708</v>
       </c>
       <c r="WN1" t="n">
-        <v>607.2689707346643</v>
+        <v>1598.6228703510096</v>
       </c>
       <c r="WO1" t="n">
-        <v>728.6970835733367</v>
+        <v>737.4361710393913</v>
       </c>
       <c r="WP1" t="n">
-        <v>730.4988858176997</v>
+        <v>707.6141482480887</v>
       </c>
       <c r="WQ1" t="n">
-        <v>918.8242425563524</v>
+        <v>685.4953002262054</v>
       </c>
       <c r="WR1" t="n">
-        <v>960.7143779276097</v>
+        <v>713.9998113131556</v>
       </c>
       <c r="WS1" t="n">
-        <v>963.5951633224458</v>
+        <v>716.7349976535003</v>
       </c>
       <c r="WT1" t="n">
-        <v>867.5793607592788</v>
+        <v>714.4480592482944</v>
       </c>
       <c r="WU1" t="n">
-        <v>864.8472405161967</v>
+        <v>719.4734752645859</v>
       </c>
       <c r="WV1" t="n">
-        <v>645.214758158041</v>
+        <v>711.5688023206646</v>
       </c>
       <c r="WW1" t="n">
-        <v>528.2113020190159</v>
+        <v>1653.679446635114</v>
       </c>
       <c r="WX1" t="n">
-        <v>460.8580079685081</v>
+        <v>1741.9011419950698</v>
       </c>
       <c r="WY1" t="n">
-        <v>431.9606781140836</v>
+        <v>1731.774835977787</v>
       </c>
       <c r="WZ1" t="n">
-        <v>389.2114520511097</v>
+        <v>1744.9071508829159</v>
       </c>
       <c r="XA1" t="n">
-        <v>329.19054258726067</v>
+        <v>1742.053572361851</v>
       </c>
       <c r="XB1" t="n">
-        <v>377.74753150915524</v>
+        <v>896.1787530972692</v>
       </c>
       <c r="XC1" t="n">
-        <v>432.57383516859124</v>
+        <v>723.1326867935157</v>
       </c>
       <c r="XD1" t="n">
-        <v>394.14571877722653</v>
+        <v>700.989342128647</v>
       </c>
       <c r="XE1" t="n">
-        <v>363.7138423408727</v>
+        <v>723.0041202300387</v>
       </c>
       <c r="XF1" t="n">
-        <v>366.2950572019159</v>
+        <v>688.4506070490745</v>
       </c>
       <c r="XG1" t="n">
-        <v>327.6827182092292</v>
+        <v>693.7440729208973</v>
       </c>
       <c r="XH1" t="n">
-        <v>259.86570059720407</v>
+        <v>738.1545423252539</v>
       </c>
       <c r="XI1" t="n">
-        <v>280.28810468453753</v>
+        <v>732.9394112756192</v>
       </c>
       <c r="XJ1" t="n">
-        <v>400.06087164214756</v>
+        <v>844.5760200015378</v>
       </c>
       <c r="XK1" t="n">
-        <v>453.60558271534444</v>
+        <v>1502.141995835102</v>
       </c>
       <c r="XL1" t="n">
-        <v>553.3662130536751</v>
+        <v>1493.9471371544746</v>
       </c>
       <c r="XM1" t="n">
-        <v>617.0007451802319</v>
+        <v>1489.4697132247718</v>
       </c>
       <c r="XN1" t="n">
-        <v>620.0313346349293</v>
+        <v>1487.841409120792</v>
       </c>
       <c r="XO1" t="n">
-        <v>550.0929606297717</v>
+        <v>1415.329207747174</v>
       </c>
       <c r="XP1" t="n">
-        <v>525.8873142326252</v>
+        <v>702.006257486811</v>
       </c>
       <c r="XQ1" t="n">
-        <v>480.534935376479</v>
+        <v>686.3522623845776</v>
       </c>
       <c r="XR1" t="n">
-        <v>403.36373495745244</v>
+        <v>698.4232707396536</v>
       </c>
       <c r="XS1" t="n">
-        <v>395.4446065405808</v>
+        <v>728.1580990860864</v>
       </c>
       <c r="XT1" t="n">
-        <v>405.99735951009797</v>
+        <v>690.3548517231264</v>
       </c>
       <c r="XU1" t="n">
-        <v>396.4646460176449</v>
+        <v>712.2019585274184</v>
       </c>
       <c r="XV1" t="n">
-        <v>336.72484228914396</v>
+        <v>676.583374286499</v>
       </c>
       <c r="XW1" t="n">
-        <v>343.812207170074</v>
+        <v>668.336711323561</v>
       </c>
       <c r="XX1" t="n">
-        <v>336.2533989746118</v>
+        <v>1652.7216117580933</v>
       </c>
       <c r="XY1" t="n">
-        <v>316.30004146926603</v>
+        <v>1653.4188264919806</v>
       </c>
       <c r="XZ1" t="n">
-        <v>291.1057134909877</v>
+        <v>1652.3983283689404</v>
       </c>
       <c r="YA1" t="n">
-        <v>261.4673982115399</v>
+        <v>1651.784350857467</v>
       </c>
       <c r="YB1" t="n">
-        <v>239.17887666759196</v>
+        <v>1651.62179747744</v>
       </c>
       <c r="YC1" t="n">
-        <v>224.57317079563379</v>
+        <v>694.5561045979165</v>
       </c>
       <c r="YD1" t="n">
-        <v>238.03379363273416</v>
+        <v>692.748140584954</v>
       </c>
       <c r="YE1" t="n">
-        <v>246.06793762374946</v>
+        <v>679.0431573657924</v>
       </c>
       <c r="YF1" t="n">
-        <v>265.62731886363287</v>
+        <v>688.835469052044</v>
       </c>
       <c r="YG1" t="n">
-        <v>317.5620975568249</v>
+        <v>674.7845153115618</v>
       </c>
       <c r="YH1" t="n">
-        <v>363.04601142729246</v>
+        <v>1886.1924775485943</v>
       </c>
       <c r="YI1" t="n">
-        <v>427.9165887956625</v>
+        <v>1893.2802852050827</v>
       </c>
       <c r="YJ1" t="n">
-        <v>496.66101554907596</v>
+        <v>1881.909431696172</v>
       </c>
       <c r="YK1" t="n">
-        <v>551.7379855996094</v>
+        <v>1899.113023232122</v>
       </c>
       <c r="YL1" t="n">
-        <v>594.3459052599725</v>
+        <v>1888.0036952523851</v>
       </c>
       <c r="YM1" t="n">
-        <v>629.8036674435128</v>
+        <v>678.9033495667335</v>
       </c>
       <c r="YN1" t="n">
-        <v>650.359201565234</v>
+        <v>724.2105800702889</v>
       </c>
       <c r="YO1" t="n">
-        <v>663.5578991527907</v>
+        <v>714.6372991434122</v>
       </c>
       <c r="YP1" t="n">
-        <v>676.8734084863238</v>
+        <v>747.5086350802075</v>
       </c>
       <c r="YQ1" t="n">
-        <v>678.2846752967737</v>
+        <v>770.5642973960055</v>
       </c>
       <c r="YR1" t="n">
-        <v>858.2999648431662</v>
+        <v>724.3109371475961</v>
       </c>
       <c r="YS1" t="n">
-        <v>879.6585726728806</v>
+        <v>666.991776771082</v>
       </c>
       <c r="YT1" t="n">
-        <v>885.1345013770874</v>
+        <v>672.8358940121126</v>
       </c>
       <c r="YU1" t="n">
-        <v>887.7163569188884</v>
+        <v>579.2935503248597</v>
       </c>
       <c r="YV1" t="n">
-        <v>859.3983001060456</v>
+        <v>540.1762969131366</v>
       </c>
       <c r="YW1" t="n">
-        <v>647.3330913611776</v>
+        <v>561.7897916201433</v>
       </c>
       <c r="YX1" t="n">
-        <v>579.3422485814515</v>
+        <v>667.7819833608319</v>
       </c>
       <c r="YY1" t="n">
-        <v>526.6091611681924</v>
+        <v>956.4855545074564</v>
       </c>
       <c r="YZ1" t="n">
-        <v>467.2004063475053</v>
+        <v>2028.1817156080488</v>
       </c>
       <c r="ZA1" t="n">
-        <v>465.0171323555941</v>
+        <v>2241.8335844529292</v>
       </c>
       <c r="ZB1" t="n">
-        <v>467.1811837165515</v>
+        <v>2252.822978028953</v>
       </c>
       <c r="ZC1" t="n">
-        <v>462.82803302739165</v>
+        <v>2226.4469374324494</v>
       </c>
       <c r="ZD1" t="n">
-        <v>472.53463847624664</v>
+        <v>2115.022114203727</v>
       </c>
       <c r="ZE1" t="n">
-        <v>494.0986370366004</v>
+        <v>1102.2786236258173</v>
       </c>
       <c r="ZF1" t="n">
-        <v>509.7931167682391</v>
+        <v>557.8641384032122</v>
       </c>
       <c r="ZG1" t="n">
-        <v>512.9325780741367</v>
+        <v>553.468219226386</v>
       </c>
       <c r="ZH1" t="n">
-        <v>518.9976252777764</v>
+        <v>546.1087545551569</v>
       </c>
       <c r="ZI1" t="n">
-        <v>516.9219261963651</v>
+        <v>545.7857301885924</v>
       </c>
       <c r="ZJ1" t="n">
-        <v>493.80810138292827</v>
+        <v>544.6428719457102</v>
       </c>
       <c r="ZK1" t="n">
-        <v>480.58937398324076</v>
+        <v>544.0880260133439</v>
       </c>
       <c r="ZL1" t="n">
-        <v>467.88740479310457</v>
+        <v>544.6196513644917</v>
       </c>
       <c r="ZM1" t="n">
-        <v>470.6592222709563</v>
+        <v>544.7387697378413</v>
       </c>
       <c r="ZN1" t="n">
-        <v>892.3855838162283</v>
+        <v>1297.1369982902372</v>
       </c>
       <c r="ZO1" t="n">
-        <v>1189.6010802217347</v>
+        <v>2876.253433383148</v>
       </c>
       <c r="ZP1" t="n">
-        <v>1040.8059376148185</v>
+        <v>2029.5163087122073</v>
       </c>
       <c r="ZQ1" t="n">
-        <v>702.0870033100327</v>
+        <v>2049.1422714423834</v>
       </c>
       <c r="ZR1" t="n">
-        <v>706.3571859806009</v>
+        <v>2120.076962794532</v>
       </c>
       <c r="ZS1" t="n">
-        <v>709.8156393186106</v>
+        <v>2145.842386819299</v>
       </c>
       <c r="ZT1" t="n">
-        <v>662.2620586689292</v>
+        <v>1186.1435026302813</v>
       </c>
       <c r="ZU1" t="n">
-        <v>520.0822786230532</v>
+        <v>1206.9648026612856</v>
       </c>
       <c r="ZV1" t="n">
-        <v>505.550995353478</v>
+        <v>1189.0451749535962</v>
       </c>
       <c r="ZW1" t="n">
-        <v>501.5954832530939</v>
+        <v>1058.3944025299952</v>
       </c>
       <c r="ZX1" t="n">
-        <v>501.9111467391527</v>
+        <v>1056.6435037773756</v>
       </c>
       <c r="ZY1" t="n">
-        <v>514.3862082928243</v>
+        <v>951.9021119037823</v>
       </c>
       <c r="ZZ1" t="n">
-        <v>530.112505135164</v>
+        <v>986.9160086343518</v>
       </c>
       <c r="AAA1" t="n">
-        <v>530.3072426042228</v>
+        <v>913.5947251139069</v>
       </c>
       <c r="AAB1" t="n">
-        <v>522.5410356493263</v>
+        <v>1746.4258562399634</v>
       </c>
       <c r="AAC1" t="n">
-        <v>512.7264642674043</v>
+        <v>1811.0974646920258</v>
       </c>
       <c r="AAD1" t="n">
-        <v>487.5120395531322</v>
+        <v>1818.0964600064387</v>
       </c>
       <c r="AAE1" t="n">
-        <v>471.43376237323304</v>
+        <v>1824.7032841514722</v>
       </c>
       <c r="AAF1" t="n">
-        <v>477.5362757494931</v>
+        <v>1823.2877773423986</v>
       </c>
       <c r="AAG1" t="n">
-        <v>487.77145697730015</v>
+        <v>1032.5149704011203</v>
       </c>
       <c r="AAH1" t="n">
-        <v>495.6391138431457</v>
+        <v>990.9070519229535</v>
       </c>
       <c r="AAI1" t="n">
-        <v>497.21495561183775</v>
+        <v>1028.340189530675</v>
       </c>
       <c r="AAJ1" t="n">
-        <v>500.6079524364231</v>
+        <v>970.7865620569464</v>
       </c>
       <c r="AAK1" t="n">
-        <v>492.59735413543643</v>
+        <v>1046.4270807035873</v>
       </c>
       <c r="AAL1" t="n">
-        <v>497.4165245992398</v>
+        <v>1028.666139974712</v>
       </c>
       <c r="AAM1" t="n">
-        <v>508.1807555114488</v>
+        <v>966.2658481539431</v>
       </c>
       <c r="AAN1" t="n">
-        <v>508.2165911387599</v>
+        <v>1030.8428786011657</v>
       </c>
       <c r="AAO1" t="n">
-        <v>506.7294241681946</v>
+        <v>1443.31402791198</v>
       </c>
       <c r="AAP1" t="n">
-        <v>566.8070209025168</v>
+        <v>1904.6323237724139</v>
       </c>
       <c r="AAQ1" t="n">
-        <v>587.8902380556206</v>
+        <v>1879.1325092181503</v>
       </c>
       <c r="AAR1" t="n">
-        <v>601.3681805441173</v>
+        <v>1900.7225501586788</v>
       </c>
       <c r="AAS1" t="n">
-        <v>606.3670617748958</v>
+        <v>1908.8703621805055</v>
       </c>
       <c r="AAT1" t="n">
-        <v>601.2507075496004</v>
+        <v>1589.2226996922113</v>
       </c>
       <c r="AAU1" t="n">
-        <v>541.7322043596587</v>
+        <v>997.1015239994395</v>
+      </c>
+      <c r="AAV1" t="n">
+        <v>987.9770580891503</v>
+      </c>
+      <c r="AAW1" t="n">
+        <v>986.0456769472443</v>
+      </c>
+      <c r="AAX1" t="n">
+        <v>993.0700230145995</v>
+      </c>
+      <c r="AAY1" t="n">
+        <v>997.1399637331906</v>
+      </c>
+      <c r="AAZ1" t="n">
+        <v>923.7168329005483</v>
+      </c>
+      <c r="ABA1" t="n">
+        <v>996.1526047491112</v>
+      </c>
+      <c r="ABB1" t="n">
+        <v>927.9794945404652</v>
+      </c>
+      <c r="ABC1" t="n">
+        <v>1823.3571468838309</v>
+      </c>
+      <c r="ABD1" t="n">
+        <v>1879.7181188320708</v>
+      </c>
+      <c r="ABE1" t="n">
+        <v>1871.4051005715548</v>
+      </c>
+      <c r="ABF1" t="n">
+        <v>1956.6989809261938</v>
+      </c>
+      <c r="ABG1" t="n">
+        <v>1944.567266590413</v>
+      </c>
+      <c r="ABH1" t="n">
+        <v>1130.2840241659737</v>
+      </c>
+      <c r="ABI1" t="n">
+        <v>1152.22541421619</v>
+      </c>
+      <c r="ABJ1" t="n">
+        <v>1157.5353787696265</v>
+      </c>
+      <c r="ABK1" t="n">
+        <v>1019.0910455660174</v>
+      </c>
+      <c r="ABL1" t="n">
+        <v>1027.5225966171686</v>
+      </c>
+      <c r="ABM1" t="n">
+        <v>992.016199601135</v>
+      </c>
+      <c r="ABN1" t="n">
+        <v>974.3807815516204</v>
+      </c>
+      <c r="ABO1" t="n">
+        <v>997.3417781270211</v>
+      </c>
+      <c r="ABP1" t="n">
+        <v>1692.8134116303402</v>
+      </c>
+      <c r="ABQ1" t="n">
+        <v>1992.0502268660894</v>
+      </c>
+      <c r="ABR1" t="n">
+        <v>1984.3176421818187</v>
+      </c>
+      <c r="ABS1" t="n">
+        <v>1993.927491296024</v>
+      </c>
+      <c r="ABT1" t="n">
+        <v>2004.4548575426788</v>
+      </c>
+      <c r="ABU1" t="n">
+        <v>1393.8943224832053</v>
+      </c>
+      <c r="ABV1" t="n">
+        <v>971.3627009643202</v>
+      </c>
+      <c r="ABW1" t="n">
+        <v>933.4584590693904</v>
+      </c>
+      <c r="ABX1" t="n">
+        <v>893.1250329633169</v>
+      </c>
+      <c r="ABY1" t="n">
+        <v>967.5251115411146</v>
+      </c>
+      <c r="ABZ1" t="n">
+        <v>976.3884316288522</v>
+      </c>
+      <c r="ACA1" t="n">
+        <v>995.3930129661916</v>
+      </c>
+      <c r="ACB1" t="n">
+        <v>1001.3953244430743</v>
+      </c>
+      <c r="ACC1" t="n">
+        <v>1584.312954875978</v>
+      </c>
+      <c r="ACD1" t="n">
+        <v>1933.986993055708</v>
+      </c>
+      <c r="ACE1" t="n">
+        <v>1949.8827380277078</v>
+      </c>
+      <c r="ACF1" t="n">
+        <v>1917.6750983419658</v>
+      </c>
+      <c r="ACG1" t="n">
+        <v>1938.0506594048481</v>
+      </c>
+      <c r="ACH1" t="n">
+        <v>1449.3543649477751</v>
+      </c>
+      <c r="ACI1" t="n">
+        <v>903.3565416153957</v>
+      </c>
+      <c r="ACJ1" t="n">
+        <v>957.2697053384197</v>
+      </c>
+      <c r="ACK1" t="n">
+        <v>910.9761869728898</v>
+      </c>
+      <c r="ACL1" t="n">
+        <v>947.2806692812336</v>
+      </c>
+      <c r="ACM1" t="n">
+        <v>894.7249028212289</v>
+      </c>
+      <c r="ACN1" t="n">
+        <v>884.4129477668148</v>
+      </c>
+      <c r="ACO1" t="n">
+        <v>832.6299740740926</v>
+      </c>
+      <c r="ACP1" t="n">
+        <v>830.3151583450627</v>
+      </c>
+      <c r="ACQ1" t="n">
+        <v>710.0807825331973</v>
+      </c>
+      <c r="ACR1" t="n">
+        <v>705.1511867557809</v>
+      </c>
+      <c r="ACS1" t="n">
+        <v>550.1989424681558</v>
+      </c>
+      <c r="ACT1" t="n">
+        <v>549.6600949809196</v>
+      </c>
+      <c r="ACU1" t="n">
+        <v>548.9359743850858</v>
+      </c>
+      <c r="ACV1" t="n">
+        <v>548.0209415433599</v>
+      </c>
+      <c r="ACW1" t="n">
+        <v>546.4904937823273</v>
+      </c>
+      <c r="ACX1" t="n">
+        <v>544.1532082571937</v>
+      </c>
+      <c r="ACY1" t="n">
+        <v>543.2494612220138</v>
+      </c>
+      <c r="ACZ1" t="n">
+        <v>543.136212231654</v>
+      </c>
+      <c r="ADA1" t="n">
+        <v>542.4917424181547</v>
+      </c>
+      <c r="ADB1" t="n">
+        <v>543.8987478187261</v>
+      </c>
+      <c r="ADC1" t="n">
+        <v>544.9739127416749</v>
+      </c>
+      <c r="ADD1" t="n">
+        <v>544.7792168238229</v>
+      </c>
+      <c r="ADE1" t="n">
+        <v>544.2469406330204</v>
+      </c>
+      <c r="ADF1" t="n">
+        <v>544.2642078887505</v>
+      </c>
+      <c r="ADG1" t="n">
+        <v>543.9718326836467</v>
+      </c>
+      <c r="ADH1" t="n">
+        <v>543.2388694920411</v>
+      </c>
+      <c r="ADI1" t="n">
+        <v>545.5222886392005</v>
+      </c>
+      <c r="ADJ1" t="n">
+        <v>545.8290375699888</v>
+      </c>
+      <c r="ADK1" t="n">
+        <v>546.9099464189485</v>
+      </c>
+      <c r="ADL1" t="n">
+        <v>546.0659813106588</v>
+      </c>
+      <c r="ADM1" t="n">
+        <v>545.7996144170892</v>
+      </c>
+      <c r="ADN1" t="n">
+        <v>543.3938289843932</v>
+      </c>
+      <c r="ADO1" t="n">
+        <v>543.0490286448749</v>
+      </c>
+      <c r="ADP1" t="n">
+        <v>542.7225719772398</v>
+      </c>
+      <c r="ADQ1" t="n">
+        <v>543.2839919490625</v>
+      </c>
+      <c r="ADR1" t="n">
+        <v>545.3902949432483</v>
+      </c>
+      <c r="ADS1" t="n">
+        <v>551.2306081403882</v>
+      </c>
+      <c r="ADT1" t="n">
+        <v>559.570664964379</v>
+      </c>
+      <c r="ADU1" t="n">
+        <v>567.3073794051518</v>
+      </c>
+      <c r="ADV1" t="n">
+        <v>577.937388604803</v>
+      </c>
+      <c r="ADW1" t="n">
+        <v>590.5808323643246</v>
+      </c>
+      <c r="ADX1" t="n">
+        <v>595.4042407742327</v>
+      </c>
+      <c r="ADY1" t="n">
+        <v>943.3785322065488</v>
+      </c>
+      <c r="ADZ1" t="n">
+        <v>1666.9553336424678</v>
+      </c>
+      <c r="AEA1" t="n">
+        <v>676.2978845378583</v>
+      </c>
+      <c r="AEB1" t="n">
+        <v>788.3233027954271</v>
+      </c>
+      <c r="AEC1" t="n">
+        <v>3027.764209779817</v>
+      </c>
+      <c r="AED1" t="n">
+        <v>3719.000411595072</v>
+      </c>
+      <c r="AEE1" t="n">
+        <v>1225.6165470037563</v>
+      </c>
+      <c r="AEF1" t="n">
+        <v>718.4586459084554</v>
+      </c>
+      <c r="AEG1" t="n">
+        <v>727.4547135408135</v>
+      </c>
+      <c r="AEH1" t="n">
+        <v>723.1236499025235</v>
+      </c>
+      <c r="AEI1" t="n">
+        <v>718.4951333711628</v>
+      </c>
+      <c r="AEJ1" t="n">
+        <v>718.2837799113438</v>
+      </c>
+      <c r="AEK1" t="n">
+        <v>688.9927045118322</v>
+      </c>
+      <c r="AEL1" t="n">
+        <v>644.3182436623808</v>
+      </c>
+      <c r="AEM1" t="n">
+        <v>641.5013947343743</v>
+      </c>
+      <c r="AEN1" t="n">
+        <v>1494.9830914302886</v>
+      </c>
+      <c r="AEO1" t="n">
+        <v>1499.627318822298</v>
+      </c>
+      <c r="AEP1" t="n">
+        <v>2334.453767836619</v>
+      </c>
+      <c r="AEQ1" t="n">
+        <v>2495.750716313551</v>
+      </c>
+      <c r="AER1" t="n">
+        <v>2495.6695631270463</v>
+      </c>
+      <c r="AES1" t="n">
+        <v>1744.1209203017</v>
+      </c>
+      <c r="AET1" t="n">
+        <v>626.5054660771253</v>
+      </c>
+      <c r="AEU1" t="n">
+        <v>618.2846640415338</v>
+      </c>
+      <c r="AEV1" t="n">
+        <v>616.8220652352574</v>
+      </c>
+      <c r="AEW1" t="n">
+        <v>611.2158729089313</v>
+      </c>
+      <c r="AEX1" t="n">
+        <v>602.400056203344</v>
+      </c>
+      <c r="AEY1" t="n">
+        <v>1200.708893131719</v>
+      </c>
+      <c r="AEZ1" t="n">
+        <v>1233.4783197874426</v>
+      </c>
+      <c r="AFA1" t="n">
+        <v>1233.6658167512314</v>
+      </c>
+      <c r="AFB1" t="n">
+        <v>1231.6470071291749</v>
+      </c>
+      <c r="AFC1" t="n">
+        <v>1236.2849666734876</v>
+      </c>
+      <c r="AFD1" t="n">
+        <v>670.3828646258813</v>
+      </c>
+      <c r="AFE1" t="n">
+        <v>617.2827182120452</v>
+      </c>
+      <c r="AFF1" t="n">
+        <v>766.9879384588063</v>
+      </c>
+      <c r="AFG1" t="n">
+        <v>2078.6795112699683</v>
+      </c>
+      <c r="AFH1" t="n">
+        <v>2144.021193701883</v>
+      </c>
+      <c r="AFI1" t="n">
+        <v>2140.664766720643</v>
+      </c>
+      <c r="AFJ1" t="n">
+        <v>2138.7467545604263</v>
+      </c>
+      <c r="AFK1" t="n">
+        <v>2095.283558757653</v>
+      </c>
+      <c r="AFL1" t="n">
+        <v>815.4935334247068</v>
+      </c>
+      <c r="AFM1" t="n">
+        <v>1124.066031310382</v>
+      </c>
+      <c r="AFN1" t="n">
+        <v>1125.1178013629756</v>
+      </c>
+      <c r="AFO1" t="n">
+        <v>1119.452801477076</v>
+      </c>
+      <c r="AFP1" t="n">
+        <v>1107.6982956743748</v>
+      </c>
+      <c r="AFQ1" t="n">
+        <v>1106.265035644116</v>
+      </c>
+      <c r="AFR1" t="n">
+        <v>587.5565039316009</v>
+      </c>
+      <c r="AFS1" t="n">
+        <v>576.493871043589</v>
+      </c>
+      <c r="AFT1" t="n">
+        <v>566.6853630317079</v>
+      </c>
+      <c r="AFU1" t="n">
+        <v>558.882743700323</v>
+      </c>
+      <c r="AFV1" t="n">
+        <v>546.7340831577031</v>
+      </c>
+      <c r="AFW1" t="n">
+        <v>538.0044943707297</v>
+      </c>
+      <c r="AFX1" t="n">
+        <v>819.2544273390951</v>
+      </c>
+      <c r="AFY1" t="n">
+        <v>1367.6688249346805</v>
+      </c>
+      <c r="AFZ1" t="n">
+        <v>1611.501067966891</v>
+      </c>
+      <c r="AGA1" t="n">
+        <v>2001.1114196549072</v>
+      </c>
+      <c r="AGB1" t="n">
+        <v>2002.172484842697</v>
+      </c>
+      <c r="AGC1" t="n">
+        <v>1906.1451559809907</v>
+      </c>
+      <c r="AGD1" t="n">
+        <v>1590.5449849827146</v>
+      </c>
+      <c r="AGE1" t="n">
+        <v>1352.7755424411998</v>
+      </c>
+      <c r="AGF1" t="n">
+        <v>663.5460622680027</v>
+      </c>
+      <c r="AGG1" t="n">
+        <v>661.1165859900044</v>
+      </c>
+      <c r="AGH1" t="n">
+        <v>658.4886391139293</v>
+      </c>
+      <c r="AGI1" t="n">
+        <v>587.3803265875495</v>
+      </c>
+      <c r="AGJ1" t="n">
+        <v>578.584881192068</v>
+      </c>
+      <c r="AGK1" t="n">
+        <v>563.575833826051</v>
+      </c>
+      <c r="AGL1" t="n">
+        <v>574.4227078805503</v>
+      </c>
+      <c r="AGM1" t="n">
+        <v>726.6576637267009</v>
+      </c>
+      <c r="AGN1" t="n">
+        <v>1176.5143129340684</v>
+      </c>
+      <c r="AGO1" t="n">
+        <v>1239.0520977173223</v>
+      </c>
+      <c r="AGP1" t="n">
+        <v>1669.953682468759</v>
+      </c>
+      <c r="AGQ1" t="n">
+        <v>1838.9105490386114</v>
+      </c>
+      <c r="AGR1" t="n">
+        <v>1854.2759178947617</v>
+      </c>
+      <c r="AGS1" t="n">
+        <v>1607.4253328742948</v>
+      </c>
+      <c r="AGT1" t="n">
+        <v>1562.5674191975866</v>
+      </c>
+      <c r="AGU1" t="n">
+        <v>1090.5857779978476</v>
+      </c>
+      <c r="AGV1" t="n">
+        <v>766.1260507290131</v>
+      </c>
+      <c r="AGW1" t="n">
+        <v>579.3935520945593</v>
+      </c>
+      <c r="AGX1" t="n">
+        <v>577.3569222022026</v>
+      </c>
+      <c r="AGY1" t="n">
+        <v>585.4327776565572</v>
+      </c>
+      <c r="AGZ1" t="n">
+        <v>602.5762769989936</v>
+      </c>
+      <c r="AHA1" t="n">
+        <v>857.9524850347017</v>
+      </c>
+      <c r="AHB1" t="n">
+        <v>996.2738415727632</v>
+      </c>
+      <c r="AHC1" t="n">
+        <v>1000.1345830774039</v>
+      </c>
+      <c r="AHD1" t="n">
+        <v>992.8107457792196</v>
+      </c>
+      <c r="AHE1" t="n">
+        <v>989.1122286926574</v>
+      </c>
+      <c r="AHF1" t="n">
+        <v>834.5719979912551</v>
+      </c>
+      <c r="AHG1" t="n">
+        <v>1377.395813608839</v>
+      </c>
+      <c r="AHH1" t="n">
+        <v>2356.171559153695</v>
+      </c>
+      <c r="AHI1" t="n">
+        <v>2412.4170944158163</v>
+      </c>
+      <c r="AHJ1" t="n">
+        <v>2518.8275579643278</v>
+      </c>
+      <c r="AHK1" t="n">
+        <v>2612.915510098032</v>
+      </c>
+      <c r="AHL1" t="n">
+        <v>2348.173257089929</v>
+      </c>
+      <c r="AHM1" t="n">
+        <v>1356.62874704897</v>
+      </c>
+      <c r="AHN1" t="n">
+        <v>1325.2451807937277</v>
+      </c>
+      <c r="AHO1" t="n">
+        <v>1280.7526845880557</v>
+      </c>
+      <c r="AHP1" t="n">
+        <v>1036.7702812009209</v>
+      </c>
+      <c r="AHQ1" t="n">
+        <v>971.27440074161</v>
+      </c>
+      <c r="AHR1" t="n">
+        <v>980.8793409109923</v>
+      </c>
+      <c r="AHS1" t="n">
+        <v>886.5723121911938</v>
+      </c>
+      <c r="AHT1" t="n">
+        <v>610.5410592259007</v>
+      </c>
+      <c r="AHU1" t="n">
+        <v>606.109654990975</v>
+      </c>
+      <c r="AHV1" t="n">
+        <v>593.0317026933733</v>
+      </c>
+      <c r="AHW1" t="n">
+        <v>588.8265957700203</v>
+      </c>
+      <c r="AHX1" t="n">
+        <v>599.0796891148475</v>
+      </c>
+      <c r="AHY1" t="n">
+        <v>609.6376378871638</v>
+      </c>
+      <c r="AHZ1" t="n">
+        <v>764.5447888917843</v>
+      </c>
+      <c r="AIA1" t="n">
+        <v>1006.1998351174676</v>
+      </c>
+      <c r="AIB1" t="n">
+        <v>1209.8511680348822</v>
+      </c>
+      <c r="AIC1" t="n">
+        <v>1348.8373970160878</v>
+      </c>
+      <c r="AID1" t="n">
+        <v>1468.6503303657278</v>
+      </c>
+      <c r="AIE1" t="n">
+        <v>1539.6111193251168</v>
+      </c>
+      <c r="AIF1" t="n">
+        <v>1395.7125934371822</v>
+      </c>
+      <c r="AIG1" t="n">
+        <v>1222.8710563932682</v>
+      </c>
+      <c r="AIH1" t="n">
+        <v>1063.8061644333884</v>
+      </c>
+      <c r="AII1" t="n">
+        <v>882.0631203814573</v>
+      </c>
+      <c r="AIJ1" t="n">
+        <v>591.6260400386636</v>
+      </c>
+      <c r="AIK1" t="n">
+        <v>612.785700243758</v>
+      </c>
+      <c r="AIL1" t="n">
+        <v>613.7088277342914</v>
+      </c>
+      <c r="AIM1" t="n">
+        <v>622.8211730491358</v>
+      </c>
+      <c r="AIN1" t="n">
+        <v>617.0884528192734</v>
+      </c>
+      <c r="AIO1" t="n">
+        <v>949.7871101304162</v>
+      </c>
+      <c r="AIP1" t="n">
+        <v>1010.9793892173649</v>
+      </c>
+      <c r="AIQ1" t="n">
+        <v>1151.9789122772925</v>
+      </c>
+      <c r="AIR1" t="n">
+        <v>1506.7685483603339</v>
+      </c>
+      <c r="AIS1" t="n">
+        <v>2130.00478757283</v>
+      </c>
+      <c r="AIT1" t="n">
+        <v>2002.437831164086</v>
+      </c>
+      <c r="AIU1" t="n">
+        <v>1961.4702388110022</v>
+      </c>
+      <c r="AIV1" t="n">
+        <v>1878.0902424500807</v>
+      </c>
+      <c r="AIW1" t="n">
+        <v>1600.5106097008918</v>
+      </c>
+      <c r="AIX1" t="n">
+        <v>554.6491389252238</v>
+      </c>
+      <c r="AIY1" t="n">
+        <v>556.3233486265722</v>
+      </c>
+      <c r="AIZ1" t="n">
+        <v>564.7146826584501</v>
+      </c>
+      <c r="AJA1" t="n">
+        <v>564.1595169979703</v>
+      </c>
+      <c r="AJB1" t="n">
+        <v>1248.9436640323058</v>
+      </c>
+      <c r="AJC1" t="n">
+        <v>1241.4754763665558</v>
+      </c>
+      <c r="AJD1" t="n">
+        <v>1239.8831776656407</v>
+      </c>
+      <c r="AJE1" t="n">
+        <v>1234.1851477599253</v>
+      </c>
+      <c r="AJF1" t="n">
+        <v>1237.6757181712915</v>
+      </c>
+      <c r="AJG1" t="n">
+        <v>533.5552058468685</v>
+      </c>
+      <c r="AJH1" t="n">
+        <v>532.4906199590806</v>
+      </c>
+      <c r="AJI1" t="n">
+        <v>2165.977009169091</v>
+      </c>
+      <c r="AJJ1" t="n">
+        <v>2691.2570029191666</v>
+      </c>
+      <c r="AJK1" t="n">
+        <v>2691.3519149655226</v>
+      </c>
+      <c r="AJL1" t="n">
+        <v>2693.2271875594</v>
+      </c>
+      <c r="AJM1" t="n">
+        <v>2696.5239942801286</v>
+      </c>
+      <c r="AJN1" t="n">
+        <v>1692.2603996857003</v>
+      </c>
+      <c r="AJO1" t="n">
+        <v>1275.4459707937717</v>
+      </c>
+      <c r="AJP1" t="n">
+        <v>1347.789241546862</v>
+      </c>
+      <c r="AJQ1" t="n">
+        <v>1365.3211817939812</v>
+      </c>
+      <c r="AJR1" t="n">
+        <v>1368.0697659631214</v>
+      </c>
+      <c r="AJS1" t="n">
+        <v>1370.624166203979</v>
+      </c>
+      <c r="AJT1" t="n">
+        <v>760.933576847373</v>
+      </c>
+      <c r="AJU1" t="n">
+        <v>640.8126879525831</v>
+      </c>
+      <c r="AJV1" t="n">
+        <v>593.3863251894654</v>
+      </c>
+      <c r="AJW1" t="n">
+        <v>577.2837206044602</v>
+      </c>
+      <c r="AJX1" t="n">
+        <v>568.9264240008904</v>
+      </c>
+      <c r="AJY1" t="n">
+        <v>557.9953989899859</v>
+      </c>
+      <c r="AJZ1" t="n">
+        <v>539.450970203654</v>
+      </c>
+      <c r="AKA1" t="n">
+        <v>2446.9874778605563</v>
+      </c>
+      <c r="AKB1" t="n">
+        <v>2792.999453760009</v>
+      </c>
+      <c r="AKC1" t="n">
+        <v>3026.037100481141</v>
+      </c>
+      <c r="AKD1" t="n">
+        <v>3025.426934297296</v>
+      </c>
+      <c r="AKE1" t="n">
+        <v>3025.775471279919</v>
+      </c>
+      <c r="AKF1" t="n">
+        <v>1881.2798208849906</v>
+      </c>
+      <c r="AKG1" t="n">
+        <v>1347.5067495178278</v>
+      </c>
+      <c r="AKH1" t="n">
+        <v>708.7528201491892</v>
+      </c>
+      <c r="AKI1" t="n">
+        <v>712.411568497586</v>
+      </c>
+      <c r="AKJ1" t="n">
+        <v>704.8682925485309</v>
+      </c>
+      <c r="AKK1" t="n">
+        <v>641.3749095120228</v>
+      </c>
+      <c r="AKL1" t="n">
+        <v>576.1792681712399</v>
+      </c>
+      <c r="AKM1" t="n">
+        <v>544.0312120667277</v>
+      </c>
+      <c r="AKN1" t="n">
+        <v>547.9344172486651</v>
+      </c>
+      <c r="AKO1" t="n">
+        <v>560.877508300899</v>
+      </c>
+      <c r="AKP1" t="n">
+        <v>1248.2790231913123</v>
+      </c>
+      <c r="AKQ1" t="n">
+        <v>1261.2711198613424</v>
+      </c>
+      <c r="AKR1" t="n">
+        <v>2883.1308737603003</v>
+      </c>
+      <c r="AKS1" t="n">
+        <v>3779.868357403402</v>
+      </c>
+      <c r="AKT1" t="n">
+        <v>526.8179810750605</v>
+      </c>
+      <c r="AKU1" t="n">
+        <v>528.9014357345244</v>
+      </c>
+      <c r="AKV1" t="n">
+        <v>538.9822631213741</v>
+      </c>
+      <c r="AKW1" t="n">
+        <v>1141.683220359949</v>
+      </c>
+      <c r="AKX1" t="n">
+        <v>1310.2366775778194</v>
+      </c>
+      <c r="AKY1" t="n">
+        <v>1794.306906582553</v>
+      </c>
+      <c r="AKZ1" t="n">
+        <v>1969.6579804802225</v>
+      </c>
+      <c r="ALA1" t="n">
+        <v>1982.716455666519</v>
+      </c>
+      <c r="ALB1" t="n">
+        <v>1707.414214465192</v>
+      </c>
+      <c r="ALC1" t="n">
+        <v>1586.6089249957056</v>
+      </c>
+      <c r="ALD1" t="n">
+        <v>989.0234765900811</v>
+      </c>
+      <c r="ALE1" t="n">
+        <v>561.0413365647165</v>
+      </c>
+      <c r="ALF1" t="n">
+        <v>2160.4819583660183</v>
+      </c>
+      <c r="ALG1" t="n">
+        <v>3576.077630462997</v>
+      </c>
+      <c r="ALH1" t="n">
+        <v>735.8838329619697</v>
+      </c>
+      <c r="ALI1" t="n">
+        <v>1532.7619954148847</v>
+      </c>
+      <c r="ALJ1" t="n">
+        <v>1519.4352260238873</v>
+      </c>
+      <c r="ALK1" t="n">
+        <v>1524.0175197755175</v>
+      </c>
+      <c r="ALL1" t="n">
+        <v>1526.8968771203863</v>
+      </c>
+      <c r="ALM1" t="n">
+        <v>1499.6683104204506</v>
+      </c>
+      <c r="ALN1" t="n">
+        <v>585.3306311710666</v>
+      </c>
+      <c r="ALO1" t="n">
+        <v>666.0123277745734</v>
+      </c>
+      <c r="ALP1" t="n">
+        <v>690.4400747528343</v>
+      </c>
+      <c r="ALQ1" t="n">
+        <v>682.5703201960955</v>
+      </c>
+      <c r="ALR1" t="n">
+        <v>673.6393476496725</v>
+      </c>
+      <c r="ALS1" t="n">
+        <v>661.1577373466162</v>
+      </c>
+      <c r="ALT1" t="n">
+        <v>1905.073754748579</v>
+      </c>
+      <c r="ALU1" t="n">
+        <v>3576.934650133429</v>
+      </c>
+      <c r="ALV1" t="n">
+        <v>1501.562144110831</v>
+      </c>
+      <c r="ALW1" t="n">
+        <v>567.7894752535932</v>
+      </c>
+      <c r="ALX1" t="n">
+        <v>584.4807475906081</v>
+      </c>
+      <c r="ALY1" t="n">
+        <v>580.282764786998</v>
+      </c>
+      <c r="ALZ1" t="n">
+        <v>573.4694498680295</v>
+      </c>
+      <c r="AMA1" t="n">
+        <v>595.689956539816</v>
+      </c>
+      <c r="AMB1" t="n">
+        <v>580.9210298562023</v>
+      </c>
+      <c r="AMC1" t="n">
+        <v>565.2850898853583</v>
+      </c>
+      <c r="AMD1" t="n">
+        <v>564.5336086244076</v>
+      </c>
+      <c r="AME1" t="n">
+        <v>1255.9430475229426</v>
+      </c>
+      <c r="AMF1" t="n">
+        <v>1400.2726757619607</v>
+      </c>
+      <c r="AMG1" t="n">
+        <v>1600.4974390102634</v>
+      </c>
+      <c r="AMH1" t="n">
+        <v>535.8022280006625</v>
+      </c>
+      <c r="AMI1" t="n">
+        <v>539.2349258508114</v>
+      </c>
+      <c r="AMJ1" t="n">
+        <v>576.234850689519</v>
+      </c>
+      <c r="AMK1" t="n">
+        <v>587.7866639089779</v>
+      </c>
+      <c r="AML1" t="n">
+        <v>600.1854831202232</v>
+      </c>
+      <c r="AMM1" t="n">
+        <v>618.5261784246902</v>
+      </c>
+      <c r="AMN1" t="n">
+        <v>1484.7724913557781</v>
+      </c>
+      <c r="AMO1" t="n">
+        <v>1508.6123853026918</v>
+      </c>
+      <c r="AMP1" t="n">
+        <v>1519.4444797596848</v>
+      </c>
+      <c r="AMQ1" t="n">
+        <v>1519.6788950698626</v>
+      </c>
+      <c r="AMR1" t="n">
+        <v>1507.448215950536</v>
+      </c>
+      <c r="AMS1" t="n">
+        <v>657.6646765618491</v>
+      </c>
+      <c r="AMT1" t="n">
+        <v>601.8009772048849</v>
+      </c>
+      <c r="AMU1" t="n">
+        <v>746.5257066216011</v>
+      </c>
+      <c r="AMV1" t="n">
+        <v>1206.8692280738742</v>
+      </c>
+      <c r="AMW1" t="n">
+        <v>1281.374064136522</v>
+      </c>
+      <c r="AMX1" t="n">
+        <v>1286.3606740403168</v>
+      </c>
+      <c r="AMY1" t="n">
+        <v>1274.6835670797227</v>
+      </c>
+      <c r="AMZ1" t="n">
+        <v>1269.5015683054935</v>
+      </c>
+      <c r="ANA1" t="n">
+        <v>732.1794731947131</v>
+      </c>
+      <c r="ANB1" t="n">
+        <v>571.3982809300479</v>
+      </c>
+      <c r="ANC1" t="n">
+        <v>580.0334056214335</v>
+      </c>
+      <c r="AND1" t="n">
+        <v>577.2139960906999</v>
+      </c>
+      <c r="ANE1" t="n">
+        <v>594.442559843272</v>
+      </c>
+      <c r="ANF1" t="n">
+        <v>590.4591534970383</v>
+      </c>
+      <c r="ANG1" t="n">
+        <v>571.1330305815068</v>
+      </c>
+      <c r="ANH1" t="n">
+        <v>1686.861424829325</v>
+      </c>
+      <c r="ANI1" t="n">
+        <v>724.3895828055014</v>
+      </c>
+      <c r="ANJ1" t="n">
+        <v>540.8902488130068</v>
+      </c>
+      <c r="ANK1" t="n">
+        <v>532.8801359244211</v>
+      </c>
+      <c r="ANL1" t="n">
+        <v>522.0193297197445</v>
+      </c>
+      <c r="ANM1" t="n">
+        <v>521.3016116752759</v>
+      </c>
+      <c r="ANN1" t="n">
+        <v>570.0631793468722</v>
+      </c>
+      <c r="ANO1" t="n">
+        <v>610.0671125315794</v>
+      </c>
+      <c r="ANP1" t="n">
+        <v>608.832083575268</v>
+      </c>
+      <c r="ANQ1" t="n">
+        <v>739.6487300372934</v>
+      </c>
+      <c r="ANR1" t="n">
+        <v>1454.6708602544638</v>
+      </c>
+      <c r="ANS1" t="n">
+        <v>1456.8574585312826</v>
+      </c>
+      <c r="ANT1" t="n">
+        <v>1021.9635877734949</v>
+      </c>
+      <c r="ANU1" t="n">
+        <v>573.4854720483747</v>
+      </c>
+      <c r="ANV1" t="n">
+        <v>564.7622221656379</v>
+      </c>
+      <c r="ANW1" t="n">
+        <v>542.0239458452111</v>
+      </c>
+      <c r="ANX1" t="n">
+        <v>535.55122158407</v>
+      </c>
+      <c r="ANY1" t="n">
+        <v>527.7615980163199</v>
+      </c>
+      <c r="ANZ1" t="n">
+        <v>1451.4472691425995</v>
+      </c>
+      <c r="AOA1" t="n">
+        <v>1459.396526598448</v>
+      </c>
+      <c r="AOB1" t="n">
+        <v>1470.069120517074</v>
+      </c>
+      <c r="AOC1" t="n">
+        <v>1472.66266642727</v>
+      </c>
+      <c r="AOD1" t="n">
+        <v>1468.8219379689901</v>
+      </c>
+      <c r="AOE1" t="n">
+        <v>535.739833021008</v>
+      </c>
+      <c r="AOF1" t="n">
+        <v>530.0545836304337</v>
+      </c>
+      <c r="AOG1" t="n">
+        <v>2234.8352447257744</v>
+      </c>
+      <c r="AOH1" t="n">
+        <v>3586.5790233557104</v>
+      </c>
+      <c r="AOI1" t="n">
+        <v>1199.3066623026743</v>
+      </c>
+      <c r="AOJ1" t="n">
+        <v>1435.096602501457</v>
+      </c>
+      <c r="AOK1" t="n">
+        <v>1457.6501914700627</v>
+      </c>
+      <c r="AOL1" t="n">
+        <v>1461.7479639197722</v>
+      </c>
+      <c r="AOM1" t="n">
+        <v>1459.6055818821558</v>
+      </c>
+      <c r="AON1" t="n">
+        <v>980.1903087050638</v>
+      </c>
+      <c r="AOO1" t="n">
+        <v>590.0843203085572</v>
+      </c>
+      <c r="AOP1" t="n">
+        <v>580.1757027363328</v>
+      </c>
+      <c r="AOQ1" t="n">
+        <v>588.8771220953973</v>
+      </c>
+      <c r="AOR1" t="n">
+        <v>606.1414431978765</v>
+      </c>
+      <c r="AOS1" t="n">
+        <v>579.250693355035</v>
+      </c>
+      <c r="AOT1" t="n">
+        <v>572.9736526509882</v>
+      </c>
+      <c r="AOU1" t="n">
+        <v>2946.569602690131</v>
+      </c>
+      <c r="AOV1" t="n">
+        <v>3677.672437967528</v>
+      </c>
+      <c r="AOW1" t="n">
+        <v>1156.1578723069326</v>
+      </c>
+      <c r="AOX1" t="n">
+        <v>531.5951757025255</v>
+      </c>
+      <c r="AOY1" t="n">
+        <v>537.3089224331359</v>
       </c>
     </row>
   </sheetData>
@@ -2256,10 +3360,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>737.4213517386108</v>
+        <v>2123.367137355196</v>
       </c>
       <c r="B1" t="n">
-        <v>737.4213517386108</v>
+        <v>857.0093348383085</v>
+      </c>
+      <c r="C1" t="n">
+        <v>1610.3682808600026</v>
+      </c>
+      <c r="D1" t="n">
+        <v>1534.4676601349408</v>
       </c>
     </row>
   </sheetData>
@@ -2277,28 +3387,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1040.4927994104523</v>
+        <v>2809.225777460758</v>
       </c>
       <c r="B1" t="n">
-        <v>987.171345625976</v>
+        <v>2594.904471989287</v>
       </c>
       <c r="C1" t="n">
-        <v>1032.1488582685154</v>
+        <v>1456.2192378725122</v>
       </c>
       <c r="D1" t="n">
-        <v>847.0242119473327</v>
+        <v>1649.5606138453961</v>
       </c>
       <c r="E1" t="n">
-        <v>1050.8048180442456</v>
+        <v>1330.5454591069033</v>
       </c>
       <c r="F1" t="n">
-        <v>855.7131620028991</v>
+        <v>1482.4604442446348</v>
       </c>
       <c r="G1" t="n">
-        <v>741.2713845987851</v>
+        <v>1300.5913919252273</v>
       </c>
       <c r="H1" t="n">
-        <v>1041.690940550507</v>
+        <v>1281.249670731665</v>
       </c>
     </row>
   </sheetData>
@@ -2316,31 +3426,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>913.1853759583524</v>
+        <v>3582.398788749328</v>
       </c>
       <c r="B1" t="n">
-        <v>751.6930355890537</v>
+        <v>1516.863520154503</v>
       </c>
       <c r="C1" t="n">
-        <v>664.8014555554478</v>
+        <v>1125.4602595908784</v>
       </c>
       <c r="D1" t="n">
-        <v>1084.9891334723525</v>
+        <v>1190.4179080971385</v>
       </c>
       <c r="E1" t="n">
-        <v>945.165992345482</v>
+        <v>1520.091706417204</v>
       </c>
       <c r="F1" t="n">
-        <v>1092.5309442745915</v>
+        <v>1129.2130996803908</v>
       </c>
       <c r="G1" t="n">
-        <v>804.8760275676536</v>
-      </c>
-      <c r="H1" t="n">
-        <v>771.9832164106634</v>
-      </c>
-      <c r="I1" t="n">
-        <v>784.8412279476785</v>
+        <v>1322.6862046299445</v>
       </c>
     </row>
   </sheetData>
@@ -2358,31 +3462,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>874.1120573981856</v>
+        <v>1770.7163804517086</v>
       </c>
       <c r="B1" t="n">
-        <v>937.0792685549903</v>
-      </c>
-      <c r="C1" t="n">
-        <v>745.5585527344955</v>
-      </c>
-      <c r="D1" t="n">
-        <v>616.60414097431</v>
-      </c>
-      <c r="E1" t="n">
-        <v>1136.5510205099558</v>
-      </c>
-      <c r="F1" t="n">
-        <v>895.6497331236383</v>
-      </c>
-      <c r="G1" t="n">
-        <v>780.5734359359719</v>
-      </c>
-      <c r="H1" t="n">
-        <v>737.9878800570583</v>
-      </c>
-      <c r="I1" t="n">
-        <v>720.8596719658179</v>
+        <v>1770.7163804517086</v>
       </c>
     </row>
   </sheetData>
@@ -2400,34 +3483,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>892.1002858423486</v>
+        <v>2877.223599344514</v>
       </c>
       <c r="B1" t="n">
-        <v>975.4792258167264</v>
+        <v>2782.676255086998</v>
       </c>
       <c r="C1" t="n">
-        <v>741.7067614630462</v>
+        <v>1582.4548621129766</v>
       </c>
       <c r="D1" t="n">
-        <v>628.3920114068924</v>
+        <v>1300.283965380255</v>
       </c>
       <c r="E1" t="n">
-        <v>1113.0317695375995</v>
+        <v>1378.3068927582856</v>
       </c>
       <c r="F1" t="n">
-        <v>907.7482690702308</v>
+        <v>1366.9660349200342</v>
       </c>
       <c r="G1" t="n">
-        <v>1116.4280182797277</v>
+        <v>1313.5930270159781</v>
       </c>
       <c r="H1" t="n">
-        <v>823.9021301101242</v>
-      </c>
-      <c r="I1" t="n">
-        <v>758.3556685355493</v>
-      </c>
-      <c r="J1" t="n">
-        <v>724.0707976434348</v>
+        <v>1393.9471441288583</v>
       </c>
     </row>
   </sheetData>
@@ -2445,22 +3522,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>886.3500844599848</v>
+        <v>1956.3293789361976</v>
       </c>
       <c r="B1" t="n">
-        <v>956.3669826774425</v>
+        <v>2603.9751609585082</v>
       </c>
       <c r="C1" t="n">
-        <v>1031.7117518420002</v>
+        <v>1859.0198955961234</v>
       </c>
       <c r="D1" t="n">
-        <v>1027.256608101836</v>
+        <v>1061.608200901925</v>
       </c>
       <c r="E1" t="n">
-        <v>781.3881700040142</v>
+        <v>1974.0978459933426</v>
       </c>
       <c r="F1" t="n">
-        <v>728.2466195519818</v>
+        <v>1658.9649299755824</v>
       </c>
     </row>
   </sheetData>
@@ -2478,67 +3555,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1101.5441748568223</v>
+        <v>1991.1236353780112</v>
       </c>
       <c r="B1" t="n">
-        <v>1107.1058355305329</v>
+        <v>2135.740068232381</v>
       </c>
       <c r="C1" t="n">
-        <v>1084.9480336991558</v>
+        <v>1438.8010047817409</v>
       </c>
       <c r="D1" t="n">
-        <v>814.8856464437482</v>
+        <v>2832.1181025419055</v>
       </c>
       <c r="E1" t="n">
-        <v>847.3302035941493</v>
+        <v>1515.3340659276907</v>
       </c>
       <c r="F1" t="n">
-        <v>896.6886955794889</v>
+        <v>1496.4247984829685</v>
       </c>
       <c r="G1" t="n">
-        <v>726.6000390724221</v>
+        <v>1652.9183121816884</v>
       </c>
       <c r="H1" t="n">
-        <v>1074.5835949307673</v>
+        <v>1477.3543741247602</v>
       </c>
       <c r="I1" t="n">
-        <v>1038.9737599780383</v>
+        <v>1957.0776744086165</v>
       </c>
       <c r="J1" t="n">
-        <v>1044.8302425885577</v>
+        <v>2850.622392332706</v>
       </c>
       <c r="K1" t="n">
-        <v>1006.3442550326346</v>
+        <v>2644.85439918711</v>
       </c>
       <c r="L1" t="n">
-        <v>921.3919064933629</v>
+        <v>1460.863925314067</v>
       </c>
       <c r="M1" t="n">
-        <v>950.639031999527</v>
-      </c>
-      <c r="N1" t="n">
-        <v>983.9982566859546</v>
-      </c>
-      <c r="O1" t="n">
-        <v>956.0739150639764</v>
-      </c>
-      <c r="P1" t="n">
-        <v>762.719475123342</v>
-      </c>
-      <c r="Q1" t="n">
-        <v>804.4603323370611</v>
-      </c>
-      <c r="R1" t="n">
-        <v>790.0860095548655</v>
-      </c>
-      <c r="S1" t="n">
-        <v>1055.8496906098887</v>
-      </c>
-      <c r="T1" t="n">
-        <v>1106.9394518732172</v>
-      </c>
-      <c r="U1" t="n">
-        <v>1134.201417242671</v>
+        <v>1472.2278332171988</v>
       </c>
     </row>
   </sheetData>
@@ -2556,16 +3609,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>831.0869012925183</v>
+        <v>2071.2365485380947</v>
       </c>
       <c r="B1" t="n">
-        <v>932.908590109449</v>
+        <v>2307.363049023712</v>
       </c>
       <c r="C1" t="n">
-        <v>853.2411367837348</v>
+        <v>846.4116256290434</v>
       </c>
       <c r="D1" t="n">
-        <v>931.6742657710365</v>
+        <v>1279.5353219040107</v>
+      </c>
+      <c r="E1" t="n">
+        <v>1597.0837298025424</v>
       </c>
     </row>
   </sheetData>
@@ -2583,37 +3639,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>926.5398083886766</v>
+        <v>2790.3269409694626</v>
       </c>
       <c r="B1" t="n">
-        <v>850.565596947551</v>
+        <v>1634.4124135297063</v>
       </c>
       <c r="C1" t="n">
-        <v>452.10851290151186</v>
+        <v>1169.8367140332023</v>
       </c>
       <c r="D1" t="n">
-        <v>892.2381552140856</v>
-      </c>
-      <c r="E1" t="n">
-        <v>1332.6020405008794</v>
-      </c>
-      <c r="F1" t="n">
-        <v>837.4820585225139</v>
-      </c>
-      <c r="G1" t="n">
-        <v>580.244320156932</v>
-      </c>
-      <c r="H1" t="n">
-        <v>530.1468220149603</v>
-      </c>
-      <c r="I1" t="n">
-        <v>483.55193213798674</v>
-      </c>
-      <c r="J1" t="n">
-        <v>540.3678193279919</v>
-      </c>
-      <c r="K1" t="n">
-        <v>648.3483338325711</v>
+        <v>1643.190475112365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>